<commit_message>
EV, ETB EV working. STDDev And weight STDDev in progress
</commit_message>
<xml_diff>
--- a/excelDocs/prismaticEvolution/pokemon_data.xlsx
+++ b/excelDocs/prismaticEvolution/pokemon_data.xlsx
@@ -673,7 +673,7 @@
         <v>0.04</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F2" s="3">
         <f>IF(B2:B210="common", 4, IF(B2:B210="uncommon", 3, IF(B2:B210="rare", 0.792892156862745, 1)))</f>
@@ -693,20 +693,20 @@
         <v/>
       </c>
       <c r="I2" s="3" t="n">
-        <v>11.1</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>65.25</v>
+        <v>60.24</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>113.65</v>
+        <v>97.33</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>5.02</v>
+        <v>5.38</v>
       </c>
       <c r="M2" s="3" t="n"/>
       <c r="N2" s="3" t="n">
-        <v>217.84</v>
+        <v>197.25</v>
       </c>
       <c r="R2" s="3" t="n"/>
       <c r="S2" s="3" t="n"/>
@@ -744,7 +744,7 @@
         <v>302</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="E3" s="3" t="inlineStr"/>
       <c r="F3" s="3">
@@ -803,7 +803,7 @@
         <v>161</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.58</v>
       </c>
       <c r="E4" s="3" t="inlineStr"/>
       <c r="F4" s="3">
@@ -862,7 +862,7 @@
         <v>1440</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>32.18</v>
+        <v>30.81</v>
       </c>
       <c r="E5" s="3" t="inlineStr"/>
       <c r="F5" s="3">
@@ -916,10 +916,10 @@
         <v>46</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F6" s="3">
         <f>IF(B6:B214="common", 4, IF(B6:B214="uncommon", 3, IF(B6:B214="rare", 0.792892156862745, 1)))</f>
@@ -972,7 +972,7 @@
         <v>1362</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>3.12</v>
+        <v>3.29</v>
       </c>
       <c r="E7" s="3" t="inlineStr"/>
       <c r="F7" s="3">
@@ -1029,7 +1029,7 @@
         <v>302</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0.46</v>
+        <v>0.43</v>
       </c>
       <c r="E8" s="3" t="inlineStr"/>
       <c r="F8" s="3">
@@ -1086,10 +1086,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.09</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F9" s="3">
         <f>IF(B9:B217="common", 4, IF(B9:B217="uncommon", 3, IF(B9:B217="rare", 0.792892156862745, 1)))</f>
@@ -1142,7 +1142,7 @@
         <v>1362</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>5.96</v>
+        <v>5.4</v>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
       <c r="F10" s="3">
@@ -1196,7 +1196,7 @@
         <v>302</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3">
@@ -1250,10 +1250,10 @@
         <v>33</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F12" s="3">
         <f>IF(B12:B220="common", 4, IF(B12:B220="uncommon", 3, IF(B12:B220="rare", 0.792892156862745, 1)))</f>
@@ -1306,7 +1306,7 @@
         <v>302</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="E13" s="3" t="inlineStr"/>
       <c r="F13" s="3">
@@ -1359,7 +1359,7 @@
         <v>0.05</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="F14" s="3">
         <f>IF(B14:B222="common", 4, IF(B14:B222="uncommon", 3, IF(B14:B222="rare", 0.792892156862745, 1)))</f>
@@ -1408,7 +1408,7 @@
         <v>1362</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>6.17</v>
+        <v>5.86</v>
       </c>
       <c r="E15" s="3" t="inlineStr"/>
       <c r="F15" s="3">
@@ -1459,7 +1459,7 @@
         <v>302</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>0.36</v>
+        <v>0.28</v>
       </c>
       <c r="E16" s="3" t="inlineStr"/>
       <c r="F16" s="3">
@@ -1510,7 +1510,7 @@
         <v>161</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>0.82</v>
+        <v>0.75</v>
       </c>
       <c r="E17" s="3" t="inlineStr"/>
       <c r="F17" s="3">
@@ -1561,7 +1561,7 @@
         <v>161</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>0.68</v>
+        <v>0.59</v>
       </c>
       <c r="E18" s="3" t="inlineStr"/>
       <c r="F18" s="3">
@@ -1615,7 +1615,7 @@
         <v>0.09</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0.19</v>
+        <v>0.14</v>
       </c>
       <c r="F19" s="3">
         <f>IF(B19:B227="common", 4, IF(B19:B227="uncommon", 3, IF(B19:B227="rare", 0.792892156862745, 1)))</f>
@@ -1665,7 +1665,7 @@
         <v>302</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
       <c r="F20" s="3">
@@ -1716,10 +1716,10 @@
         <v>46</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="F21" s="3">
         <f>IF(B21:B229="common", 4, IF(B21:B229="uncommon", 3, IF(B21:B229="rare", 0.792892156862745, 1)))</f>
@@ -1769,7 +1769,7 @@
         <v>302</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>0.45</v>
+        <v>0.34</v>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
       <c r="F22" s="3">
@@ -1823,7 +1823,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="F23" s="3">
         <f>IF(B23:B231="common", 4, IF(B23:B231="uncommon", 3, IF(B23:B231="rare", 0.792892156862745, 1)))</f>
@@ -1873,7 +1873,7 @@
         <v>302</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
       <c r="F24" s="3">
@@ -1924,10 +1924,10 @@
         <v>46</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F25" s="3">
         <f>IF(B25:B233="common", 4, IF(B25:B233="uncommon", 3, IF(B25:B233="rare", 0.792892156862745, 1)))</f>
@@ -1977,7 +1977,7 @@
         <v>302</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>0.31</v>
+        <v>0.34</v>
       </c>
       <c r="E26" s="3" t="inlineStr"/>
       <c r="F26" s="3">
@@ -2031,7 +2031,7 @@
         <v>0.04</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F27" s="3">
         <f>IF(B27:B235="common", 4, IF(B27:B235="uncommon", 3, IF(B27:B235="rare", 0.792892156862745, 1)))</f>
@@ -2081,7 +2081,7 @@
         <v>302</v>
       </c>
       <c r="D28" s="3" t="n">
-        <v>0.36</v>
+        <v>0.33</v>
       </c>
       <c r="E28" s="3" t="inlineStr"/>
       <c r="F28" s="3">
@@ -2132,7 +2132,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>0.13</v>
@@ -2185,7 +2185,7 @@
         <v>1362</v>
       </c>
       <c r="D30" s="3" t="n">
-        <v>8.83</v>
+        <v>8.66</v>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
       <c r="F30" s="3">
@@ -2236,7 +2236,7 @@
         <v>302</v>
       </c>
       <c r="D31" s="3" t="n">
-        <v>0.44</v>
+        <v>0.36</v>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
       <c r="F31" s="3">
@@ -2287,7 +2287,7 @@
         <v>1440</v>
       </c>
       <c r="D32" s="3" t="n">
-        <v>108.9</v>
+        <v>105.71</v>
       </c>
       <c r="E32" s="3" t="inlineStr"/>
       <c r="F32" s="3">
@@ -2338,7 +2338,7 @@
         <v>161</v>
       </c>
       <c r="D33" s="3" t="n">
-        <v>0.73</v>
+        <v>0.54</v>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
       <c r="F33" s="3">
@@ -2389,10 +2389,10 @@
         <v>33</v>
       </c>
       <c r="D34" s="3" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F34" s="3">
         <f>IF(B34:B242="common", 4, IF(B34:B242="uncommon", 3, IF(B34:B242="rare", 0.792892156862745, 1)))</f>
@@ -2442,7 +2442,7 @@
         <v>302</v>
       </c>
       <c r="D35" s="3" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
       <c r="F35" s="3">
@@ -2493,10 +2493,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="E36" s="3" t="n">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F36" s="3">
         <f>IF(B36:B244="common", 4, IF(B36:B244="uncommon", 3, IF(B36:B244="rare", 0.792892156862745, 1)))</f>
@@ -2546,7 +2546,7 @@
         <v>1362</v>
       </c>
       <c r="D37" s="3" t="n">
-        <v>7.11</v>
+        <v>6.76</v>
       </c>
       <c r="E37" s="3" t="inlineStr"/>
       <c r="F37" s="3">
@@ -2597,7 +2597,7 @@
         <v>302</v>
       </c>
       <c r="D38" s="3" t="n">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="E38" s="3" t="inlineStr"/>
       <c r="F38" s="3">
@@ -2651,7 +2651,7 @@
         <v>0.03</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F39" s="3">
         <f>IF(B39:B247="common", 4, IF(B39:B247="uncommon", 3, IF(B39:B247="rare", 0.792892156862745, 1)))</f>
@@ -2701,7 +2701,7 @@
         <v>1362</v>
       </c>
       <c r="D40" s="3" t="n">
-        <v>1.7</v>
+        <v>1.42</v>
       </c>
       <c r="E40" s="3" t="inlineStr"/>
       <c r="F40" s="3">
@@ -2752,7 +2752,7 @@
         <v>302</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="E41" s="3" t="inlineStr"/>
       <c r="F41" s="3">
@@ -2803,10 +2803,10 @@
         <v>33</v>
       </c>
       <c r="D42" s="3" t="n">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
       <c r="E42" s="3" t="n">
-        <v>0.37</v>
+        <v>0.33</v>
       </c>
       <c r="F42" s="3">
         <f>IF(B42:B250="common", 4, IF(B42:B250="uncommon", 3, IF(B42:B250="rare", 0.792892156862745, 1)))</f>
@@ -2856,7 +2856,7 @@
         <v>302</v>
       </c>
       <c r="D43" s="3" t="n">
-        <v>2.15</v>
+        <v>2.01</v>
       </c>
       <c r="E43" s="3" t="inlineStr"/>
       <c r="F43" s="3">
@@ -2907,10 +2907,10 @@
         <v>46</v>
       </c>
       <c r="D44" s="3" t="n">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="E44" s="3" t="n">
-        <v>0.42</v>
+        <v>0.47</v>
       </c>
       <c r="F44" s="3">
         <f>IF(B44:B252="common", 4, IF(B44:B252="uncommon", 3, IF(B44:B252="rare", 0.792892156862745, 1)))</f>
@@ -2960,7 +2960,7 @@
         <v>1362</v>
       </c>
       <c r="D45" s="3" t="n">
-        <v>13.21</v>
+        <v>13.15</v>
       </c>
       <c r="E45" s="3" t="inlineStr"/>
       <c r="F45" s="3">
@@ -3011,7 +3011,7 @@
         <v>302</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>3.65</v>
+        <v>3.28</v>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
       <c r="F46" s="3">
@@ -3062,10 +3062,10 @@
         <v>33</v>
       </c>
       <c r="D47" s="3" t="n">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="F47" s="3">
         <f>IF(B47:B255="common", 4, IF(B47:B255="uncommon", 3, IF(B47:B255="rare", 0.792892156862745, 1)))</f>
@@ -3115,7 +3115,7 @@
         <v>302</v>
       </c>
       <c r="D48" s="3" t="n">
-        <v>0.62</v>
+        <v>0.46</v>
       </c>
       <c r="E48" s="3" t="inlineStr"/>
       <c r="F48" s="3">
@@ -3169,7 +3169,7 @@
         <v>0.04</v>
       </c>
       <c r="E49" s="3" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F49" s="3">
         <f>IF(B49:B257="common", 4, IF(B49:B257="uncommon", 3, IF(B49:B257="rare", 0.792892156862745, 1)))</f>
@@ -3219,7 +3219,7 @@
         <v>1362</v>
       </c>
       <c r="D50" s="3" t="n">
-        <v>2.15</v>
+        <v>2.19</v>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
       <c r="F50" s="3">
@@ -3270,7 +3270,7 @@
         <v>302</v>
       </c>
       <c r="D51" s="3" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="E51" s="3" t="inlineStr"/>
       <c r="F51" s="3">
@@ -3321,10 +3321,10 @@
         <v>33</v>
       </c>
       <c r="D52" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E52" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F52" s="3">
         <f>IF(B52:B260="common", 4, IF(B52:B260="uncommon", 3, IF(B52:B260="rare", 0.792892156862745, 1)))</f>
@@ -3374,7 +3374,7 @@
         <v>302</v>
       </c>
       <c r="D53" s="3" t="n">
-        <v>0.39</v>
+        <v>0.51</v>
       </c>
       <c r="E53" s="3" t="inlineStr"/>
       <c r="F53" s="3">
@@ -3425,7 +3425,7 @@
         <v>1440</v>
       </c>
       <c r="D54" s="3" t="n">
-        <v>167.46</v>
+        <v>144.29</v>
       </c>
       <c r="E54" s="3" t="inlineStr"/>
       <c r="F54" s="3">
@@ -3476,10 +3476,10 @@
         <v>33</v>
       </c>
       <c r="D55" s="3" t="n">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E55" s="3" t="n">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="F55" s="3">
         <f>IF(B55:B263="common", 4, IF(B55:B263="uncommon", 3, IF(B55:B263="rare", 0.792892156862745, 1)))</f>
@@ -3529,7 +3529,7 @@
         <v>302</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>0.59</v>
+        <v>0.46</v>
       </c>
       <c r="E56" s="3" t="inlineStr"/>
       <c r="F56" s="3">
@@ -3580,7 +3580,7 @@
         <v>106</v>
       </c>
       <c r="D57" s="3" t="n">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="E57" s="3" t="inlineStr"/>
       <c r="F57" s="3">
@@ -3631,7 +3631,7 @@
         <v>1440</v>
       </c>
       <c r="D58" s="3" t="n">
-        <v>21.92</v>
+        <v>20.35</v>
       </c>
       <c r="E58" s="3" t="inlineStr"/>
       <c r="F58" s="3">
@@ -3685,7 +3685,7 @@
         <v>0.03</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="F59" s="3">
         <f>IF(B59:B267="common", 4, IF(B59:B267="uncommon", 3, IF(B59:B267="rare", 0.792892156862745, 1)))</f>
@@ -3735,7 +3735,7 @@
         <v>1362</v>
       </c>
       <c r="D60" s="3" t="n">
-        <v>1.63</v>
+        <v>1.7</v>
       </c>
       <c r="E60" s="3" t="inlineStr"/>
       <c r="F60" s="3">
@@ -3786,7 +3786,7 @@
         <v>302</v>
       </c>
       <c r="D61" s="3" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
       <c r="F61" s="3">
@@ -3837,10 +3837,10 @@
         <v>33</v>
       </c>
       <c r="D62" s="3" t="n">
-        <v>0.34</v>
+        <v>0.27</v>
       </c>
       <c r="E62" s="3" t="n">
-        <v>0.39</v>
+        <v>0.31</v>
       </c>
       <c r="F62" s="3">
         <f>IF(B62:B270="common", 4, IF(B62:B270="uncommon", 3, IF(B62:B270="rare", 0.792892156862745, 1)))</f>
@@ -3890,7 +3890,7 @@
         <v>302</v>
       </c>
       <c r="D63" s="3" t="n">
-        <v>1.69</v>
+        <v>1.54</v>
       </c>
       <c r="E63" s="3" t="inlineStr"/>
       <c r="F63" s="3">
@@ -3941,7 +3941,7 @@
         <v>1440</v>
       </c>
       <c r="D64" s="3" t="n">
-        <v>47.92</v>
+        <v>45.24</v>
       </c>
       <c r="E64" s="3" t="inlineStr"/>
       <c r="F64" s="3">
@@ -3992,10 +3992,10 @@
         <v>33</v>
       </c>
       <c r="D65" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E65" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F65" s="3">
         <f>IF(B65:B273="common", 4, IF(B65:B273="uncommon", 3, IF(B65:B273="rare", 0.792892156862745, 1)))</f>
@@ -4045,7 +4045,7 @@
         <v>1362</v>
       </c>
       <c r="D66" s="3" t="n">
-        <v>3.07</v>
+        <v>2.58</v>
       </c>
       <c r="E66" s="3" t="inlineStr"/>
       <c r="F66" s="3">
@@ -4096,7 +4096,7 @@
         <v>302</v>
       </c>
       <c r="D67" s="3" t="n">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="E67" s="3" t="inlineStr"/>
       <c r="F67" s="3">
@@ -4147,7 +4147,7 @@
         <v>106</v>
       </c>
       <c r="D68" s="3" t="n">
-        <v>1.65</v>
+        <v>1.57</v>
       </c>
       <c r="E68" s="3" t="inlineStr"/>
       <c r="F68" s="3">
@@ -4198,7 +4198,7 @@
         <v>1440</v>
       </c>
       <c r="D69" s="3" t="n">
-        <v>133.93</v>
+        <v>127.32</v>
       </c>
       <c r="E69" s="3" t="inlineStr"/>
       <c r="F69" s="3">
@@ -4249,10 +4249,10 @@
         <v>46</v>
       </c>
       <c r="D70" s="3" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="E70" s="3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="F70" s="3">
         <f>IF(B70:B278="common", 4, IF(B70:B278="uncommon", 3, IF(B70:B278="rare", 0.792892156862745, 1)))</f>
@@ -4302,7 +4302,7 @@
         <v>1362</v>
       </c>
       <c r="D71" s="3" t="n">
-        <v>10.27</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E71" s="3" t="inlineStr"/>
       <c r="F71" s="3">
@@ -4353,7 +4353,7 @@
         <v>302</v>
       </c>
       <c r="D72" s="3" t="n">
-        <v>1.79</v>
+        <v>1.09</v>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
       <c r="F72" s="3">
@@ -4404,7 +4404,7 @@
         <v>1440</v>
       </c>
       <c r="D73" s="3" t="n">
-        <v>32.9</v>
+        <v>31.42</v>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
       <c r="F73" s="3">
@@ -4455,10 +4455,10 @@
         <v>46</v>
       </c>
       <c r="D74" s="3" t="n">
-        <v>0.08</v>
+        <v>0.13</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="F74" s="3">
         <f>IF(B74:B282="common", 4, IF(B74:B282="uncommon", 3, IF(B74:B282="rare", 0.792892156862745, 1)))</f>
@@ -4508,7 +4508,7 @@
         <v>1362</v>
       </c>
       <c r="D75" s="3" t="n">
-        <v>8.44</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="E75" s="3" t="inlineStr"/>
       <c r="F75" s="3">
@@ -4559,7 +4559,7 @@
         <v>302</v>
       </c>
       <c r="D76" s="3" t="n">
-        <v>2.63</v>
+        <v>1.93</v>
       </c>
       <c r="E76" s="3" t="inlineStr"/>
       <c r="F76" s="3">
@@ -4610,10 +4610,10 @@
         <v>21</v>
       </c>
       <c r="D77" s="3" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="F77" s="3">
         <f>IF(B77:B285="common", 4, IF(B77:B285="uncommon", 3, IF(B77:B285="rare", 0.792892156862745, 1)))</f>
@@ -4663,7 +4663,7 @@
         <v>1362</v>
       </c>
       <c r="D78" s="3" t="n">
-        <v>15.08</v>
+        <v>15.09</v>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
       <c r="F78" s="3">
@@ -4714,7 +4714,7 @@
         <v>302</v>
       </c>
       <c r="D79" s="3" t="n">
-        <v>0.92</v>
+        <v>0.79</v>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
       <c r="F79" s="3">
@@ -4768,7 +4768,7 @@
         <v>0.04</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F80" s="3">
         <f>IF(B80:B288="common", 4, IF(B80:B288="uncommon", 3, IF(B80:B288="rare", 0.792892156862745, 1)))</f>
@@ -4818,7 +4818,7 @@
         <v>1362</v>
       </c>
       <c r="D81" s="3" t="n">
-        <v>2.89</v>
+        <v>2.66</v>
       </c>
       <c r="E81" s="3" t="inlineStr"/>
       <c r="F81" s="3">
@@ -4869,7 +4869,7 @@
         <v>302</v>
       </c>
       <c r="D82" s="3" t="n">
-        <v>0.5</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E82" s="3" t="inlineStr"/>
       <c r="F82" s="3">
@@ -4973,7 +4973,7 @@
         <v>1362</v>
       </c>
       <c r="D84" s="3" t="n">
-        <v>5.13</v>
+        <v>4.57</v>
       </c>
       <c r="E84" s="3" t="inlineStr"/>
       <c r="F84" s="3">
@@ -5024,7 +5024,7 @@
         <v>302</v>
       </c>
       <c r="D85" s="3" t="n">
-        <v>0.99</v>
+        <v>0.78</v>
       </c>
       <c r="E85" s="3" t="inlineStr"/>
       <c r="F85" s="3">
@@ -5075,10 +5075,10 @@
         <v>46</v>
       </c>
       <c r="D86" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E86" s="3" t="n">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="F86" s="3">
         <f>IF(B86:B294="common", 4, IF(B86:B294="uncommon", 3, IF(B86:B294="rare", 0.792892156862745, 1)))</f>
@@ -5128,7 +5128,7 @@
         <v>1362</v>
       </c>
       <c r="D87" s="3" t="n">
-        <v>3.25</v>
+        <v>3.07</v>
       </c>
       <c r="E87" s="3" t="inlineStr"/>
       <c r="F87" s="3">
@@ -5179,7 +5179,7 @@
         <v>302</v>
       </c>
       <c r="D88" s="3" t="n">
-        <v>0.76</v>
+        <v>0.49</v>
       </c>
       <c r="E88" s="3" t="inlineStr"/>
       <c r="F88" s="3">
@@ -5230,10 +5230,10 @@
         <v>21</v>
       </c>
       <c r="D89" s="3" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E89" s="3" t="n">
-        <v>0.32</v>
+        <v>0.23</v>
       </c>
       <c r="F89" s="3">
         <f>IF(B89:B297="common", 4, IF(B89:B297="uncommon", 3, IF(B89:B297="rare", 0.792892156862745, 1)))</f>
@@ -5283,7 +5283,7 @@
         <v>1362</v>
       </c>
       <c r="D90" s="3" t="n">
-        <v>9.529999999999999</v>
+        <v>9.06</v>
       </c>
       <c r="E90" s="3" t="inlineStr"/>
       <c r="F90" s="3">
@@ -5334,7 +5334,7 @@
         <v>302</v>
       </c>
       <c r="D91" s="3" t="n">
-        <v>1.18</v>
+        <v>0.79</v>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
       <c r="F91" s="3">
@@ -5388,7 +5388,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E92" s="3" t="n">
-        <v>0.11</v>
+        <v>0.14</v>
       </c>
       <c r="F92" s="3">
         <f>IF(B92:B300="common", 4, IF(B92:B300="uncommon", 3, IF(B92:B300="rare", 0.792892156862745, 1)))</f>
@@ -5438,7 +5438,7 @@
         <v>1362</v>
       </c>
       <c r="D93" s="3" t="n">
-        <v>4.26</v>
+        <v>3.9</v>
       </c>
       <c r="E93" s="3" t="inlineStr"/>
       <c r="F93" s="3">
@@ -5489,7 +5489,7 @@
         <v>302</v>
       </c>
       <c r="D94" s="3" t="n">
-        <v>0.82</v>
+        <v>0.68</v>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
       <c r="F94" s="3">
@@ -5540,10 +5540,10 @@
         <v>33</v>
       </c>
       <c r="D95" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="F95" s="3">
         <f>IF(B95:B303="common", 4, IF(B95:B303="uncommon", 3, IF(B95:B303="rare", 0.792892156862745, 1)))</f>
@@ -5593,7 +5593,7 @@
         <v>302</v>
       </c>
       <c r="D96" s="3" t="n">
-        <v>1.24</v>
+        <v>1.19</v>
       </c>
       <c r="E96" s="3" t="inlineStr"/>
       <c r="F96" s="3">
@@ -5644,10 +5644,10 @@
         <v>46</v>
       </c>
       <c r="D97" s="3" t="n">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="E97" s="3" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="F97" s="3">
         <f>IF(B97:B305="common", 4, IF(B97:B305="uncommon", 3, IF(B97:B305="rare", 0.792892156862745, 1)))</f>
@@ -5697,7 +5697,7 @@
         <v>1362</v>
       </c>
       <c r="D98" s="3" t="n">
-        <v>12.23</v>
+        <v>11.4</v>
       </c>
       <c r="E98" s="3" t="inlineStr"/>
       <c r="F98" s="3">
@@ -5748,7 +5748,7 @@
         <v>302</v>
       </c>
       <c r="D99" s="3" t="n">
-        <v>1.41</v>
+        <v>1.63</v>
       </c>
       <c r="E99" s="3" t="inlineStr"/>
       <c r="F99" s="3">
@@ -5799,7 +5799,7 @@
         <v>106</v>
       </c>
       <c r="D100" s="3" t="n">
-        <v>5.6</v>
+        <v>4.38</v>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
       <c r="F100" s="3">
@@ -5850,7 +5850,7 @@
         <v>1440</v>
       </c>
       <c r="D101" s="3" t="n">
-        <v>167.92</v>
+        <v>147.41</v>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
       <c r="F101" s="3">
@@ -5901,7 +5901,7 @@
         <v>161</v>
       </c>
       <c r="D102" s="3" t="n">
-        <v>2.04</v>
+        <v>1.63</v>
       </c>
       <c r="E102" s="3" t="inlineStr"/>
       <c r="F102" s="3">
@@ -5952,10 +5952,10 @@
         <v>21</v>
       </c>
       <c r="D103" s="3" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E103" s="3" t="n">
-        <v>0.37</v>
+        <v>0.32</v>
       </c>
       <c r="F103" s="3">
         <f>IF(B103:B311="common", 4, IF(B103:B311="uncommon", 3, IF(B103:B311="rare", 0.792892156862745, 1)))</f>
@@ -6005,7 +6005,7 @@
         <v>1362</v>
       </c>
       <c r="D104" s="3" t="n">
-        <v>41.3</v>
+        <v>35.86</v>
       </c>
       <c r="E104" s="3" t="inlineStr"/>
       <c r="F104" s="3">
@@ -6056,7 +6056,7 @@
         <v>302</v>
       </c>
       <c r="D105" s="3" t="n">
-        <v>1.84</v>
+        <v>1.8</v>
       </c>
       <c r="E105" s="3" t="inlineStr"/>
       <c r="F105" s="3">
@@ -6107,7 +6107,7 @@
         <v>106</v>
       </c>
       <c r="D106" s="3" t="n">
-        <v>3.06</v>
+        <v>2.48</v>
       </c>
       <c r="E106" s="3" t="inlineStr"/>
       <c r="F106" s="3">
@@ -6158,7 +6158,7 @@
         <v>1440</v>
       </c>
       <c r="D107" s="3" t="n">
-        <v>341.41</v>
+        <v>321.31</v>
       </c>
       <c r="E107" s="3" t="inlineStr"/>
       <c r="F107" s="3">
@@ -6209,10 +6209,10 @@
         <v>46</v>
       </c>
       <c r="D108" s="3" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E108" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="F108" s="3">
         <f>IF(B108:B316="common", 4, IF(B108:B316="uncommon", 3, IF(B108:B316="rare", 0.792892156862745, 1)))</f>
@@ -6262,7 +6262,7 @@
         <v>1362</v>
       </c>
       <c r="D109" s="3" t="n">
-        <v>2.98</v>
+        <v>2.63</v>
       </c>
       <c r="E109" s="3" t="inlineStr"/>
       <c r="F109" s="3">
@@ -6313,7 +6313,7 @@
         <v>302</v>
       </c>
       <c r="D110" s="3" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="E110" s="3" t="inlineStr"/>
       <c r="F110" s="3">
@@ -6364,10 +6364,10 @@
         <v>33</v>
       </c>
       <c r="D111" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E111" s="3" t="n">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F111" s="3">
         <f>IF(B111:B319="common", 4, IF(B111:B319="uncommon", 3, IF(B111:B319="rare", 0.792892156862745, 1)))</f>
@@ -6417,7 +6417,7 @@
         <v>1362</v>
       </c>
       <c r="D112" s="3" t="n">
-        <v>9.970000000000001</v>
+        <v>9.779999999999999</v>
       </c>
       <c r="E112" s="3" t="inlineStr"/>
       <c r="F112" s="3">
@@ -6468,7 +6468,7 @@
         <v>302</v>
       </c>
       <c r="D113" s="3" t="n">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E113" s="3" t="inlineStr"/>
       <c r="F113" s="3">
@@ -6519,7 +6519,7 @@
         <v>33</v>
       </c>
       <c r="D114" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="E114" s="3" t="n">
         <v>0.13</v>
@@ -6572,7 +6572,7 @@
         <v>302</v>
       </c>
       <c r="D115" s="3" t="n">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="E115" s="3" t="inlineStr"/>
       <c r="F115" s="3">
@@ -6623,10 +6623,10 @@
         <v>46</v>
       </c>
       <c r="D116" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="E116" s="3" t="n">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="F116" s="3">
         <f>IF(B116:B324="common", 4, IF(B116:B324="uncommon", 3, IF(B116:B324="rare", 0.792892156862745, 1)))</f>
@@ -6676,7 +6676,7 @@
         <v>1362</v>
       </c>
       <c r="D117" s="3" t="n">
-        <v>6.87</v>
+        <v>5.56</v>
       </c>
       <c r="E117" s="3" t="inlineStr"/>
       <c r="F117" s="3">
@@ -6727,7 +6727,7 @@
         <v>302</v>
       </c>
       <c r="D118" s="3" t="n">
-        <v>0.97</v>
+        <v>0.86</v>
       </c>
       <c r="E118" s="3" t="inlineStr"/>
       <c r="F118" s="3">
@@ -6778,10 +6778,10 @@
         <v>33</v>
       </c>
       <c r="D119" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E119" s="3" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="F119" s="3">
         <f>IF(B119:B327="common", 4, IF(B119:B327="uncommon", 3, IF(B119:B327="rare", 0.792892156862745, 1)))</f>
@@ -6831,7 +6831,7 @@
         <v>302</v>
       </c>
       <c r="D120" s="3" t="n">
-        <v>0.34</v>
+        <v>0.29</v>
       </c>
       <c r="E120" s="3" t="inlineStr"/>
       <c r="F120" s="3">
@@ -6882,10 +6882,10 @@
         <v>21</v>
       </c>
       <c r="D121" s="3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E121" s="3" t="n">
         <v>0.08</v>
-      </c>
-      <c r="E121" s="3" t="n">
-        <v>0.11</v>
       </c>
       <c r="F121" s="3">
         <f>IF(B121:B329="common", 4, IF(B121:B329="uncommon", 3, IF(B121:B329="rare", 0.792892156862745, 1)))</f>
@@ -6935,7 +6935,7 @@
         <v>1362</v>
       </c>
       <c r="D122" s="3" t="n">
-        <v>7.14</v>
+        <v>7.56</v>
       </c>
       <c r="E122" s="3" t="inlineStr"/>
       <c r="F122" s="3">
@@ -6986,7 +6986,7 @@
         <v>302</v>
       </c>
       <c r="D123" s="3" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="E123" s="3" t="inlineStr"/>
       <c r="F123" s="3">
@@ -7037,10 +7037,10 @@
         <v>21</v>
       </c>
       <c r="D124" s="3" t="n">
-        <v>0.17</v>
+        <v>0.14</v>
       </c>
       <c r="E124" s="3" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="F124" s="3">
         <f>IF(B124:B332="common", 4, IF(B124:B332="uncommon", 3, IF(B124:B332="rare", 0.792892156862745, 1)))</f>
@@ -7090,7 +7090,7 @@
         <v>1362</v>
       </c>
       <c r="D125" s="3" t="n">
-        <v>35.29</v>
+        <v>33.82</v>
       </c>
       <c r="E125" s="3" t="inlineStr"/>
       <c r="F125" s="3">
@@ -7141,7 +7141,7 @@
         <v>302</v>
       </c>
       <c r="D126" s="3" t="n">
-        <v>1.53</v>
+        <v>1.33</v>
       </c>
       <c r="E126" s="3" t="inlineStr"/>
       <c r="F126" s="3">
@@ -7192,7 +7192,7 @@
         <v>106</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>9.81</v>
+        <v>7.98</v>
       </c>
       <c r="E127" s="3" t="inlineStr"/>
       <c r="F127" s="3">
@@ -7243,7 +7243,7 @@
         <v>1440</v>
       </c>
       <c r="D128" s="3" t="n">
-        <v>264.89</v>
+        <v>255.29</v>
       </c>
       <c r="E128" s="3" t="inlineStr"/>
       <c r="F128" s="3">
@@ -7294,10 +7294,10 @@
         <v>21</v>
       </c>
       <c r="D129" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E129" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F129" s="3">
         <f>IF(B129:B337="common", 4, IF(B129:B337="uncommon", 3, IF(B129:B337="rare", 0.792892156862745, 1)))</f>
@@ -7347,7 +7347,7 @@
         <v>1362</v>
       </c>
       <c r="D130" s="3" t="n">
-        <v>9.460000000000001</v>
+        <v>9.34</v>
       </c>
       <c r="E130" s="3" t="inlineStr"/>
       <c r="F130" s="3">
@@ -7398,7 +7398,7 @@
         <v>302</v>
       </c>
       <c r="D131" s="3" t="n">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="E131" s="3" t="inlineStr"/>
       <c r="F131" s="3">
@@ -7449,10 +7449,10 @@
         <v>46</v>
       </c>
       <c r="D132" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E132" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F132" s="3">
         <f>IF(B132:B340="common", 4, IF(B132:B340="uncommon", 3, IF(B132:B340="rare", 0.792892156862745, 1)))</f>
@@ -7502,7 +7502,7 @@
         <v>302</v>
       </c>
       <c r="D133" s="3" t="n">
-        <v>0.26</v>
+        <v>0.18</v>
       </c>
       <c r="E133" s="3" t="inlineStr"/>
       <c r="F133" s="3">
@@ -7553,7 +7553,7 @@
         <v>161</v>
       </c>
       <c r="D134" s="3" t="n">
-        <v>1.48</v>
+        <v>1.27</v>
       </c>
       <c r="E134" s="3" t="inlineStr"/>
       <c r="F134" s="3">
@@ -7657,7 +7657,7 @@
         <v>1362</v>
       </c>
       <c r="D136" s="3" t="n">
-        <v>7.11</v>
+        <v>7.06</v>
       </c>
       <c r="E136" s="3" t="inlineStr"/>
       <c r="F136" s="3">
@@ -7708,7 +7708,7 @@
         <v>302</v>
       </c>
       <c r="D137" s="3" t="n">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="E137" s="3" t="inlineStr"/>
       <c r="F137" s="3">
@@ -7759,7 +7759,7 @@
         <v>1440</v>
       </c>
       <c r="D138" s="3" t="n">
-        <v>86.73</v>
+        <v>84.88</v>
       </c>
       <c r="E138" s="3" t="inlineStr"/>
       <c r="F138" s="3">
@@ -7810,7 +7810,7 @@
         <v>161</v>
       </c>
       <c r="D139" s="3" t="n">
-        <v>0.61</v>
+        <v>0.64</v>
       </c>
       <c r="E139" s="3" t="inlineStr"/>
       <c r="F139" s="3">
@@ -7861,10 +7861,10 @@
         <v>21</v>
       </c>
       <c r="D140" s="3" t="n">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="E140" s="3" t="n">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="F140" s="3">
         <f>IF(B140:B348="common", 4, IF(B140:B348="uncommon", 3, IF(B140:B348="rare", 0.792892156862745, 1)))</f>
@@ -7914,7 +7914,7 @@
         <v>1362</v>
       </c>
       <c r="D141" s="3" t="n">
-        <v>32.98</v>
+        <v>33.96</v>
       </c>
       <c r="E141" s="3" t="inlineStr"/>
       <c r="F141" s="3">
@@ -7965,7 +7965,7 @@
         <v>302</v>
       </c>
       <c r="D142" s="3" t="n">
-        <v>1.22</v>
+        <v>1.56</v>
       </c>
       <c r="E142" s="3" t="inlineStr"/>
       <c r="F142" s="3">
@@ -8016,7 +8016,7 @@
         <v>106</v>
       </c>
       <c r="D143" s="3" t="n">
-        <v>1.85</v>
+        <v>1.57</v>
       </c>
       <c r="E143" s="3" t="inlineStr"/>
       <c r="F143" s="3">
@@ -8067,7 +8067,7 @@
         <v>1440</v>
       </c>
       <c r="D144" s="3" t="n">
-        <v>272.53</v>
+        <v>247.26</v>
       </c>
       <c r="E144" s="3" t="inlineStr"/>
       <c r="F144" s="3">
@@ -8118,7 +8118,7 @@
         <v>33</v>
       </c>
       <c r="D145" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E145" s="3" t="n">
         <v>0.14</v>
@@ -8171,7 +8171,7 @@
         <v>302</v>
       </c>
       <c r="D146" s="3" t="n">
-        <v>0.55</v>
+        <v>0.45</v>
       </c>
       <c r="E146" s="3" t="inlineStr"/>
       <c r="F146" s="3">
@@ -8222,10 +8222,10 @@
         <v>46</v>
       </c>
       <c r="D147" s="3" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E147" s="3" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="F147" s="3">
         <f>IF(B147:B355="common", 4, IF(B147:B355="uncommon", 3, IF(B147:B355="rare", 0.792892156862745, 1)))</f>
@@ -8275,7 +8275,7 @@
         <v>1362</v>
       </c>
       <c r="D148" s="3" t="n">
-        <v>3.5</v>
+        <v>3.36</v>
       </c>
       <c r="E148" s="3" t="inlineStr"/>
       <c r="F148" s="3">
@@ -8326,7 +8326,7 @@
         <v>302</v>
       </c>
       <c r="D149" s="3" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="E149" s="3" t="inlineStr"/>
       <c r="F149" s="3">
@@ -8377,7 +8377,7 @@
         <v>33</v>
       </c>
       <c r="D150" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E150" s="3" t="n">
         <v>0.15</v>
@@ -8430,7 +8430,7 @@
         <v>1362</v>
       </c>
       <c r="D151" s="3" t="n">
-        <v>7.35</v>
+        <v>7.29</v>
       </c>
       <c r="E151" s="3" t="inlineStr"/>
       <c r="F151" s="3">
@@ -8481,7 +8481,7 @@
         <v>302</v>
       </c>
       <c r="D152" s="3" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="E152" s="3" t="inlineStr"/>
       <c r="F152" s="3">
@@ -8532,10 +8532,10 @@
         <v>21</v>
       </c>
       <c r="D153" s="3" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="E153" s="3" t="n">
-        <v>0.13</v>
+        <v>0.16</v>
       </c>
       <c r="F153" s="3">
         <f>IF(B153:B361="common", 4, IF(B153:B361="uncommon", 3, IF(B153:B361="rare", 0.792892156862745, 1)))</f>
@@ -8585,7 +8585,7 @@
         <v>1362</v>
       </c>
       <c r="D154" s="3" t="n">
-        <v>14.43</v>
+        <v>14</v>
       </c>
       <c r="E154" s="3" t="inlineStr"/>
       <c r="F154" s="3">
@@ -8636,7 +8636,7 @@
         <v>302</v>
       </c>
       <c r="D155" s="3" t="n">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="E155" s="3" t="inlineStr"/>
       <c r="F155" s="3">
@@ -8690,7 +8690,7 @@
         <v>0.06</v>
       </c>
       <c r="E156" s="3" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="F156" s="3">
         <f>IF(B156:B364="common", 4, IF(B156:B364="uncommon", 3, IF(B156:B364="rare", 0.792892156862745, 1)))</f>
@@ -8740,7 +8740,7 @@
         <v>302</v>
       </c>
       <c r="D157" s="3" t="n">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="E157" s="3" t="inlineStr"/>
       <c r="F157" s="3">
@@ -8791,10 +8791,10 @@
         <v>33</v>
       </c>
       <c r="D158" s="3" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E158" s="3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F158" s="3">
         <f>IF(B158:B366="common", 4, IF(B158:B366="uncommon", 3, IF(B158:B366="rare", 0.792892156862745, 1)))</f>
@@ -8844,7 +8844,7 @@
         <v>1362</v>
       </c>
       <c r="D159" s="3" t="n">
-        <v>2.65</v>
+        <v>1.72</v>
       </c>
       <c r="E159" s="3" t="inlineStr"/>
       <c r="F159" s="3">
@@ -8895,7 +8895,7 @@
         <v>302</v>
       </c>
       <c r="D160" s="3" t="n">
-        <v>0.35</v>
+        <v>0.22</v>
       </c>
       <c r="E160" s="3" t="inlineStr"/>
       <c r="F160" s="3">
@@ -8946,7 +8946,7 @@
         <v>106</v>
       </c>
       <c r="D161" s="3" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E161" s="3" t="inlineStr"/>
       <c r="F161" s="3">
@@ -8997,7 +8997,7 @@
         <v>1440</v>
       </c>
       <c r="D162" s="3" t="n">
-        <v>24.1</v>
+        <v>22.79</v>
       </c>
       <c r="E162" s="3" t="inlineStr"/>
       <c r="F162" s="3">
@@ -9051,7 +9051,7 @@
         <v>0.04</v>
       </c>
       <c r="E163" s="3" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F163" s="3">
         <f>IF(B163:B371="common", 4, IF(B163:B371="uncommon", 3, IF(B163:B371="rare", 0.792892156862745, 1)))</f>
@@ -9101,7 +9101,7 @@
         <v>1362</v>
       </c>
       <c r="D164" s="3" t="n">
-        <v>2.08</v>
+        <v>1.75</v>
       </c>
       <c r="E164" s="3" t="inlineStr"/>
       <c r="F164" s="3">
@@ -9152,7 +9152,7 @@
         <v>302</v>
       </c>
       <c r="D165" s="3" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="E165" s="3" t="inlineStr"/>
       <c r="F165" s="3">
@@ -9206,7 +9206,7 @@
         <v>0.04</v>
       </c>
       <c r="E166" s="3" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F166" s="3">
         <f>IF(B166:B374="common", 4, IF(B166:B374="uncommon", 3, IF(B166:B374="rare", 0.792892156862745, 1)))</f>
@@ -9256,7 +9256,7 @@
         <v>1362</v>
       </c>
       <c r="D167" s="3" t="n">
-        <v>2.9</v>
+        <v>2.57</v>
       </c>
       <c r="E167" s="3" t="inlineStr"/>
       <c r="F167" s="3">
@@ -9307,7 +9307,7 @@
         <v>302</v>
       </c>
       <c r="D168" s="3" t="n">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="E168" s="3" t="inlineStr"/>
       <c r="F168" s="3">
@@ -9358,10 +9358,10 @@
         <v>46</v>
       </c>
       <c r="D169" s="3" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E169" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F169" s="3">
         <f>IF(B169:B377="common", 4, IF(B169:B377="uncommon", 3, IF(B169:B377="rare", 0.792892156862745, 1)))</f>
@@ -9411,7 +9411,7 @@
         <v>1362</v>
       </c>
       <c r="D170" s="3" t="n">
-        <v>6.85</v>
+        <v>5.48</v>
       </c>
       <c r="E170" s="3" t="inlineStr"/>
       <c r="F170" s="3">
@@ -9462,7 +9462,7 @@
         <v>302</v>
       </c>
       <c r="D171" s="3" t="n">
-        <v>0.33</v>
+        <v>0.24</v>
       </c>
       <c r="E171" s="3" t="inlineStr"/>
       <c r="F171" s="3">
@@ -9513,10 +9513,10 @@
         <v>46</v>
       </c>
       <c r="D172" s="3" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="E172" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F172" s="3">
         <f>IF(B172:B380="common", 4, IF(B172:B380="uncommon", 3, IF(B172:B380="rare", 0.792892156862745, 1)))</f>
@@ -9566,7 +9566,7 @@
         <v>1362</v>
       </c>
       <c r="D173" s="3" t="n">
-        <v>4.63</v>
+        <v>4.11</v>
       </c>
       <c r="E173" s="3" t="inlineStr"/>
       <c r="F173" s="3">
@@ -9668,10 +9668,10 @@
         <v>46</v>
       </c>
       <c r="D175" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E175" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F175" s="3">
         <f>IF(B175:B383="common", 4, IF(B175:B383="uncommon", 3, IF(B175:B383="rare", 0.792892156862745, 1)))</f>
@@ -9721,7 +9721,7 @@
         <v>1362</v>
       </c>
       <c r="D176" s="3" t="n">
-        <v>14.77</v>
+        <v>12.94</v>
       </c>
       <c r="E176" s="3" t="inlineStr"/>
       <c r="F176" s="3">
@@ -9772,7 +9772,7 @@
         <v>302</v>
       </c>
       <c r="D177" s="3" t="n">
-        <v>0.49</v>
+        <v>0.44</v>
       </c>
       <c r="E177" s="3" t="inlineStr"/>
       <c r="F177" s="3">
@@ -9826,7 +9826,7 @@
         <v>0.03</v>
       </c>
       <c r="E178" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F178" s="3">
         <f>IF(B178:B386="common", 4, IF(B178:B386="uncommon", 3, IF(B178:B386="rare", 0.792892156862745, 1)))</f>
@@ -9876,7 +9876,7 @@
         <v>1362</v>
       </c>
       <c r="D179" s="3" t="n">
-        <v>3.11</v>
+        <v>3.06</v>
       </c>
       <c r="E179" s="3" t="inlineStr"/>
       <c r="F179" s="3">
@@ -9927,7 +9927,7 @@
         <v>302</v>
       </c>
       <c r="D180" s="3" t="n">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="E180" s="3" t="inlineStr"/>
       <c r="F180" s="3">
@@ -9978,7 +9978,7 @@
         <v>106</v>
       </c>
       <c r="D181" s="3" t="n">
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="E181" s="3" t="inlineStr"/>
       <c r="F181" s="3">
@@ -10029,10 +10029,10 @@
         <v>21</v>
       </c>
       <c r="D182" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E182" s="3" t="n">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="F182" s="3">
         <f>IF(B182:B390="common", 4, IF(B182:B390="uncommon", 3, IF(B182:B390="rare", 0.792892156862745, 1)))</f>
@@ -10082,7 +10082,7 @@
         <v>1362</v>
       </c>
       <c r="D183" s="3" t="n">
-        <v>7.96</v>
+        <v>5.87</v>
       </c>
       <c r="E183" s="3" t="inlineStr"/>
       <c r="F183" s="3">
@@ -10133,7 +10133,7 @@
         <v>302</v>
       </c>
       <c r="D184" s="3" t="n">
-        <v>0.45</v>
+        <v>0.32</v>
       </c>
       <c r="E184" s="3" t="inlineStr"/>
       <c r="F184" s="3">
@@ -10184,7 +10184,7 @@
         <v>1440</v>
       </c>
       <c r="D185" s="3" t="n">
-        <v>69.40000000000001</v>
+        <v>61.25</v>
       </c>
       <c r="E185" s="3" t="inlineStr"/>
       <c r="F185" s="3">
@@ -10235,7 +10235,7 @@
         <v>106</v>
       </c>
       <c r="D186" s="3" t="n">
-        <v>1.05</v>
+        <v>1.02</v>
       </c>
       <c r="E186" s="3" t="inlineStr"/>
       <c r="F186" s="3">
@@ -10286,7 +10286,7 @@
         <v>1440</v>
       </c>
       <c r="D187" s="3" t="n">
-        <v>52.36</v>
+        <v>49.76</v>
       </c>
       <c r="E187" s="3" t="inlineStr"/>
       <c r="F187" s="3">
@@ -10337,7 +10337,7 @@
         <v>900</v>
       </c>
       <c r="D188" s="3" t="n">
-        <v>7.84</v>
+        <v>5.87</v>
       </c>
       <c r="E188" s="3" t="inlineStr"/>
       <c r="F188" s="3">
@@ -10388,7 +10388,7 @@
         <v>106</v>
       </c>
       <c r="D189" s="3" t="n">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
       <c r="E189" s="3" t="inlineStr"/>
       <c r="F189" s="3">
@@ -10439,7 +10439,7 @@
         <v>1440</v>
       </c>
       <c r="D190" s="3" t="n">
-        <v>68.66</v>
+        <v>62.84</v>
       </c>
       <c r="E190" s="3" t="inlineStr"/>
       <c r="F190" s="3">
@@ -10490,10 +10490,10 @@
         <v>33</v>
       </c>
       <c r="D191" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E191" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="F191" s="3">
         <f>IF(B191:B399="common", 4, IF(B191:B399="uncommon", 3, IF(B191:B399="rare", 0.792892156862745, 1)))</f>
@@ -10543,7 +10543,7 @@
         <v>302</v>
       </c>
       <c r="D192" s="3" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
       <c r="E192" s="3" t="inlineStr"/>
       <c r="F192" s="3">
@@ -10594,7 +10594,7 @@
         <v>1440</v>
       </c>
       <c r="D193" s="3" t="n">
-        <v>43.06</v>
+        <v>41.58</v>
       </c>
       <c r="E193" s="3" t="inlineStr"/>
       <c r="F193" s="3">
@@ -10645,10 +10645,10 @@
         <v>21</v>
       </c>
       <c r="D194" s="3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="E194" s="3" t="n">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="F194" s="3">
         <f>IF(B194:B402="common", 4, IF(B194:B402="uncommon", 3, IF(B194:B402="rare", 0.792892156862745, 1)))</f>
@@ -10698,7 +10698,7 @@
         <v>1362</v>
       </c>
       <c r="D195" s="3" t="n">
-        <v>33.35</v>
+        <v>31.67</v>
       </c>
       <c r="E195" s="3" t="inlineStr"/>
       <c r="F195" s="3">
@@ -10749,7 +10749,7 @@
         <v>302</v>
       </c>
       <c r="D196" s="3" t="n">
-        <v>1.43</v>
+        <v>1.65</v>
       </c>
       <c r="E196" s="3" t="inlineStr"/>
       <c r="F196" s="3">
@@ -10800,7 +10800,7 @@
         <v>106</v>
       </c>
       <c r="D197" s="3" t="n">
-        <v>2.43</v>
+        <v>1.65</v>
       </c>
       <c r="E197" s="3" t="n">
         <v>7.48</v>
@@ -10853,7 +10853,7 @@
         <v>1440</v>
       </c>
       <c r="D198" s="3" t="n">
-        <v>322.67</v>
+        <v>260.7</v>
       </c>
       <c r="E198" s="3" t="inlineStr"/>
       <c r="F198" s="3">
@@ -10907,7 +10907,7 @@
         <v>0.07000000000000001</v>
       </c>
       <c r="E199" s="3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="F199" s="3">
         <f>IF(B199:B407="common", 4, IF(B199:B407="uncommon", 3, IF(B199:B407="rare", 0.792892156862745, 1)))</f>
@@ -10957,7 +10957,7 @@
         <v>302</v>
       </c>
       <c r="D200" s="3" t="n">
-        <v>0.38</v>
+        <v>0.47</v>
       </c>
       <c r="E200" s="3" t="inlineStr"/>
       <c r="F200" s="3">
@@ -11008,7 +11008,7 @@
         <v>1440</v>
       </c>
       <c r="D201" s="3" t="n">
-        <v>42.58</v>
+        <v>40.86</v>
       </c>
       <c r="E201" s="3" t="inlineStr"/>
       <c r="F201" s="3">
@@ -11062,7 +11062,7 @@
         <v>0.04</v>
       </c>
       <c r="E202" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="F202" s="3">
         <f>IF(B202:B410="common", 4, IF(B202:B410="uncommon", 3, IF(B202:B410="rare", 0.792892156862745, 1)))</f>
@@ -11112,7 +11112,7 @@
         <v>302</v>
       </c>
       <c r="D203" s="3" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E203" s="3" t="inlineStr"/>
       <c r="F203" s="3">
@@ -11163,7 +11163,7 @@
         <v>1440</v>
       </c>
       <c r="D204" s="3" t="n">
-        <v>48.14</v>
+        <v>45.41</v>
       </c>
       <c r="E204" s="3" t="inlineStr"/>
       <c r="F204" s="3">
@@ -11214,10 +11214,10 @@
         <v>46</v>
       </c>
       <c r="D205" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E205" s="3" t="n">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F205" s="3">
         <f>IF(B205:B413="common", 4, IF(B205:B413="uncommon", 3, IF(B205:B413="rare", 0.792892156862745, 1)))</f>
@@ -11267,7 +11267,7 @@
         <v>302</v>
       </c>
       <c r="D206" s="3" t="n">
-        <v>0.33</v>
+        <v>0.27</v>
       </c>
       <c r="E206" s="3" t="inlineStr"/>
       <c r="F206" s="3">
@@ -11318,7 +11318,7 @@
         <v>161</v>
       </c>
       <c r="D207" s="3" t="n">
-        <v>0.75</v>
+        <v>0.57</v>
       </c>
       <c r="E207" s="3" t="inlineStr"/>
       <c r="F207" s="3">
@@ -11369,10 +11369,10 @@
         <v>46</v>
       </c>
       <c r="D208" s="3" t="n">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="E208" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F208" s="3">
         <f>IF(B208:B416="common", 4, IF(B208:B416="uncommon", 3, IF(B208:B416="rare", 0.792892156862745, 1)))</f>
@@ -11422,7 +11422,7 @@
         <v>1362</v>
       </c>
       <c r="D209" s="3" t="n">
-        <v>3.58</v>
+        <v>3.57</v>
       </c>
       <c r="E209" s="3" t="inlineStr"/>
       <c r="F209" s="3">
@@ -11473,7 +11473,7 @@
         <v>302</v>
       </c>
       <c r="D210" s="3" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
       <c r="E210" s="3" t="inlineStr"/>
       <c r="F210" s="3">
@@ -11524,10 +11524,10 @@
         <v>21</v>
       </c>
       <c r="D211" s="3" t="n">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="E211" s="3" t="n">
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="F211" s="3">
         <f>IF(B211:B419="common", 4, IF(B211:B419="uncommon", 3, IF(B211:B419="rare", 0.792892156862745, 1)))</f>
@@ -11556,7 +11556,7 @@
         <v>1362</v>
       </c>
       <c r="D212" s="3" t="n">
-        <v>34.77</v>
+        <v>33.65</v>
       </c>
       <c r="E212" s="3" t="inlineStr"/>
       <c r="F212" s="3">
@@ -11592,7 +11592,7 @@
         <v>302</v>
       </c>
       <c r="D213" s="3" t="n">
-        <v>1.44</v>
+        <v>1.42</v>
       </c>
       <c r="E213" s="3" t="inlineStr"/>
       <c r="F213" s="3">
@@ -11622,7 +11622,7 @@
         <v>106</v>
       </c>
       <c r="D214" s="3" t="n">
-        <v>4.16</v>
+        <v>3.62</v>
       </c>
       <c r="E214" s="3" t="inlineStr"/>
       <c r="F214" s="3">
@@ -11652,7 +11652,7 @@
         <v>1440</v>
       </c>
       <c r="D215" s="3" t="n">
-        <v>363.53</v>
+        <v>345.18</v>
       </c>
       <c r="E215" s="3" t="inlineStr"/>
       <c r="F215" s="3">
@@ -11682,7 +11682,7 @@
         <v>46</v>
       </c>
       <c r="D216" s="3" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E216" s="3" t="n">
         <v>0.1</v>
@@ -11714,7 +11714,7 @@
         <v>1362</v>
       </c>
       <c r="D217" s="3" t="n">
-        <v>2.21</v>
+        <v>1.56</v>
       </c>
       <c r="E217" s="3" t="inlineStr"/>
       <c r="F217" s="3">
@@ -11744,7 +11744,7 @@
         <v>302</v>
       </c>
       <c r="D218" s="3" t="n">
-        <v>0.35</v>
+        <v>0.28</v>
       </c>
       <c r="E218" s="3" t="inlineStr"/>
       <c r="F218" s="3">
@@ -11774,10 +11774,10 @@
         <v>46</v>
       </c>
       <c r="D219" s="3" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="E219" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F219" s="3">
         <f>IF(B219:B427="common", 4, IF(B219:B427="uncommon", 3, IF(B219:B427="rare", 0.792892156862745, 1)))</f>
@@ -11806,7 +11806,7 @@
         <v>1362</v>
       </c>
       <c r="D220" s="3" t="n">
-        <v>9.59</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="E220" s="3" t="inlineStr"/>
       <c r="F220" s="3">
@@ -11836,7 +11836,7 @@
         <v>302</v>
       </c>
       <c r="D221" s="3" t="n">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="E221" s="3" t="inlineStr"/>
       <c r="F221" s="3">
@@ -11866,7 +11866,7 @@
         <v>106</v>
       </c>
       <c r="D222" s="3" t="n">
-        <v>0.64</v>
+        <v>0.55</v>
       </c>
       <c r="E222" s="3" t="inlineStr"/>
       <c r="F222" s="3">
@@ -11896,7 +11896,7 @@
         <v>106</v>
       </c>
       <c r="D223" s="3" t="n">
-        <v>0.9</v>
+        <v>0.98</v>
       </c>
       <c r="E223" s="3" t="inlineStr"/>
       <c r="F223" s="3">
@@ -11926,7 +11926,7 @@
         <v>128</v>
       </c>
       <c r="D224" s="3" t="n">
-        <v>0.64</v>
+        <v>0.74</v>
       </c>
       <c r="E224" s="3" t="inlineStr"/>
       <c r="F224" s="3">
@@ -11956,7 +11956,7 @@
         <v>128</v>
       </c>
       <c r="D225" s="3" t="n">
-        <v>0.77</v>
+        <v>0.64</v>
       </c>
       <c r="E225" s="3" t="inlineStr"/>
       <c r="F225" s="3">
@@ -11986,7 +11986,7 @@
         <v>161</v>
       </c>
       <c r="D226" s="3" t="n">
-        <v>1.18</v>
+        <v>1.24</v>
       </c>
       <c r="E226" s="3" t="inlineStr"/>
       <c r="F226" s="3">
@@ -12019,7 +12019,7 @@
         <v>0.03</v>
       </c>
       <c r="E227" s="3" t="n">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="F227" s="3">
         <f>IF(B227:B435="common", 4, IF(B227:B435="uncommon", 3, IF(B227:B435="rare", 0.792892156862745, 1)))</f>
@@ -12048,7 +12048,7 @@
         <v>1362</v>
       </c>
       <c r="D228" s="3" t="n">
-        <v>3.18</v>
+        <v>2.96</v>
       </c>
       <c r="E228" s="3" t="inlineStr"/>
       <c r="F228" s="3">
@@ -12078,7 +12078,7 @@
         <v>302</v>
       </c>
       <c r="D229" s="3" t="n">
-        <v>0.42</v>
+        <v>0.36</v>
       </c>
       <c r="E229" s="3" t="inlineStr"/>
       <c r="F229" s="3">
@@ -12108,10 +12108,10 @@
         <v>21</v>
       </c>
       <c r="D230" s="3" t="n">
-        <v>0.39</v>
+        <v>0.45</v>
       </c>
       <c r="E230" s="3" t="n">
-        <v>0.42</v>
+        <v>0.51</v>
       </c>
       <c r="F230" s="3">
         <f>IF(B230:B438="common", 4, IF(B230:B438="uncommon", 3, IF(B230:B438="rare", 0.792892156862745, 1)))</f>
@@ -12140,7 +12140,7 @@
         <v>1362</v>
       </c>
       <c r="D231" s="3" t="n">
-        <v>12.19</v>
+        <v>12.27</v>
       </c>
       <c r="E231" s="3" t="inlineStr"/>
       <c r="F231" s="3">
@@ -12170,7 +12170,7 @@
         <v>302</v>
       </c>
       <c r="D232" s="3" t="n">
-        <v>1.42</v>
+        <v>1.76</v>
       </c>
       <c r="E232" s="3" t="inlineStr"/>
       <c r="F232" s="3">
@@ -12200,10 +12200,10 @@
         <v>21</v>
       </c>
       <c r="D233" s="3" t="n">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="E233" s="3" t="n">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
       <c r="F233" s="3">
         <f>IF(B233:B441="common", 4, IF(B233:B441="uncommon", 3, IF(B233:B441="rare", 0.792892156862745, 1)))</f>
@@ -12232,7 +12232,7 @@
         <v>1362</v>
       </c>
       <c r="D234" s="3" t="n">
-        <v>10.21</v>
+        <v>9.49</v>
       </c>
       <c r="E234" s="3" t="inlineStr"/>
       <c r="F234" s="3">
@@ -12262,7 +12262,7 @@
         <v>302</v>
       </c>
       <c r="D235" s="3" t="n">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="E235" s="3" t="inlineStr"/>
       <c r="F235" s="3">
@@ -12292,7 +12292,7 @@
         <v>46</v>
       </c>
       <c r="D236" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E236" s="3" t="n">
         <v>0.14</v>
@@ -12324,7 +12324,7 @@
         <v>1362</v>
       </c>
       <c r="D237" s="3" t="n">
-        <v>2.91</v>
+        <v>2.48</v>
       </c>
       <c r="E237" s="3" t="inlineStr"/>
       <c r="F237" s="3">
@@ -12354,7 +12354,7 @@
         <v>302</v>
       </c>
       <c r="D238" s="3" t="n">
-        <v>0.38</v>
+        <v>0.29</v>
       </c>
       <c r="E238" s="3" t="inlineStr"/>
       <c r="F238" s="3">
@@ -12384,7 +12384,7 @@
         <v>106</v>
       </c>
       <c r="D239" s="3" t="n">
-        <v>0.43</v>
+        <v>0.46</v>
       </c>
       <c r="E239" s="3" t="inlineStr"/>
       <c r="F239" s="3">
@@ -12446,7 +12446,7 @@
         <v>302</v>
       </c>
       <c r="D241" s="3" t="n">
-        <v>0.39</v>
+        <v>0.29</v>
       </c>
       <c r="E241" s="3" t="inlineStr"/>
       <c r="F241" s="3">
@@ -12476,10 +12476,10 @@
         <v>21</v>
       </c>
       <c r="D242" s="3" t="n">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="E242" s="3" t="n">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F242" s="3">
         <f>IF(B242:B450="common", 4, IF(B242:B450="uncommon", 3, IF(B242:B450="rare", 0.792892156862745, 1)))</f>
@@ -12508,7 +12508,7 @@
         <v>1362</v>
       </c>
       <c r="D243" s="3" t="n">
-        <v>6.36</v>
+        <v>6.58</v>
       </c>
       <c r="E243" s="3" t="inlineStr"/>
       <c r="F243" s="3">
@@ -12538,7 +12538,7 @@
         <v>302</v>
       </c>
       <c r="D244" s="3" t="n">
-        <v>0.28</v>
+        <v>0.34</v>
       </c>
       <c r="E244" s="3" t="inlineStr"/>
       <c r="F244" s="3">
@@ -12568,7 +12568,7 @@
         <v>161</v>
       </c>
       <c r="D245" s="3" t="n">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="E245" s="3" t="inlineStr"/>
       <c r="F245" s="3">
@@ -12598,7 +12598,7 @@
         <v>1440</v>
       </c>
       <c r="D246" s="3" t="n">
-        <v>74.52</v>
+        <v>74.34</v>
       </c>
       <c r="E246" s="3" t="inlineStr"/>
       <c r="F246" s="3">
@@ -12628,7 +12628,7 @@
         <v>1440</v>
       </c>
       <c r="D247" s="3" t="n">
-        <v>37.17</v>
+        <v>33.06</v>
       </c>
       <c r="E247" s="3" t="inlineStr"/>
       <c r="F247" s="3">
@@ -12658,7 +12658,7 @@
         <v>106</v>
       </c>
       <c r="D248" s="3" t="n">
-        <v>0.97</v>
+        <v>0.78</v>
       </c>
       <c r="E248" s="3" t="inlineStr"/>
       <c r="F248" s="3">
@@ -12688,7 +12688,7 @@
         <v>900</v>
       </c>
       <c r="D249" s="3" t="n">
-        <v>44.74</v>
+        <v>40.39</v>
       </c>
       <c r="E249" s="3" t="inlineStr"/>
       <c r="F249" s="3">
@@ -12721,7 +12721,7 @@
         <v>0.03</v>
       </c>
       <c r="E250" s="3" t="n">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="F250" s="3">
         <f>IF(B250:B458="common", 4, IF(B250:B458="uncommon", 3, IF(B250:B458="rare", 0.792892156862745, 1)))</f>
@@ -12750,7 +12750,7 @@
         <v>1362</v>
       </c>
       <c r="D251" s="3" t="n">
-        <v>3.33</v>
+        <v>3.22</v>
       </c>
       <c r="E251" s="3" t="inlineStr"/>
       <c r="F251" s="3">
@@ -12780,7 +12780,7 @@
         <v>302</v>
       </c>
       <c r="D252" s="3" t="n">
-        <v>0.31</v>
+        <v>0.26</v>
       </c>
       <c r="E252" s="3" t="inlineStr"/>
       <c r="F252" s="3">
@@ -12810,7 +12810,7 @@
         <v>128</v>
       </c>
       <c r="D253" s="3" t="n">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="E253" s="3" t="inlineStr"/>
       <c r="F253" s="3">
@@ -12840,10 +12840,10 @@
         <v>33</v>
       </c>
       <c r="D254" s="3" t="n">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="E254" s="3" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="F254" s="3">
         <f>IF(B254:B462="common", 4, IF(B254:B462="uncommon", 3, IF(B254:B462="rare", 0.792892156862745, 1)))</f>
@@ -12872,7 +12872,7 @@
         <v>302</v>
       </c>
       <c r="D255" s="3" t="n">
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="E255" s="3" t="inlineStr"/>
       <c r="F255" s="3">
@@ -12905,7 +12905,7 @@
         <v>0.09</v>
       </c>
       <c r="E256" s="3" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="F256" s="3">
         <f>IF(B256:B464="common", 4, IF(B256:B464="uncommon", 3, IF(B256:B464="rare", 0.792892156862745, 1)))</f>
@@ -12934,7 +12934,7 @@
         <v>302</v>
       </c>
       <c r="D257" s="3" t="n">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
       <c r="E257" s="3" t="inlineStr"/>
       <c r="F257" s="3">
@@ -12964,10 +12964,10 @@
         <v>46</v>
       </c>
       <c r="D258" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E258" s="3" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F258" s="3">
         <f>IF(B258:B466="common", 4, IF(B258:B466="uncommon", 3, IF(B258:B466="rare", 0.792892156862745, 1)))</f>
@@ -12996,7 +12996,7 @@
         <v>302</v>
       </c>
       <c r="D259" s="3" t="n">
-        <v>0.51</v>
+        <v>0.42</v>
       </c>
       <c r="E259" s="3" t="inlineStr"/>
       <c r="F259" s="3">
@@ -13026,10 +13026,10 @@
         <v>46</v>
       </c>
       <c r="D260" s="3" t="n">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="E260" s="3" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F260" s="3">
         <f>IF(B260:B468="common", 4, IF(B260:B468="uncommon", 3, IF(B260:B468="rare", 0.792892156862745, 1)))</f>
@@ -13058,7 +13058,7 @@
         <v>302</v>
       </c>
       <c r="D261" s="3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="E261" s="3" t="inlineStr"/>
       <c r="F261" s="3">
@@ -13091,7 +13091,7 @@
         <v>0.08</v>
       </c>
       <c r="E262" s="3" t="n">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="F262" s="3">
         <f>IF(B262:B470="common", 4, IF(B262:B470="uncommon", 3, IF(B262:B470="rare", 0.792892156862745, 1)))</f>
@@ -13120,7 +13120,7 @@
         <v>302</v>
       </c>
       <c r="D263" s="3" t="n">
-        <v>0.38</v>
+        <v>0.51</v>
       </c>
       <c r="E263" s="3" t="inlineStr"/>
       <c r="F263" s="3">
@@ -13150,7 +13150,7 @@
         <v>46</v>
       </c>
       <c r="D264" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E264" s="3" t="n">
         <v>0.11</v>
@@ -13182,7 +13182,7 @@
         <v>302</v>
       </c>
       <c r="D265" s="3" t="n">
-        <v>0.49</v>
+        <v>0.37</v>
       </c>
       <c r="E265" s="3" t="inlineStr"/>
       <c r="F265" s="3">
@@ -13212,10 +13212,10 @@
         <v>46</v>
       </c>
       <c r="D266" s="3" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E266" s="3" t="n">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="F266" s="3">
         <f>IF(B266:B474="common", 4, IF(B266:B474="uncommon", 3, IF(B266:B474="rare", 0.792892156862745, 1)))</f>
@@ -13244,7 +13244,7 @@
         <v>1362</v>
       </c>
       <c r="D267" s="3" t="n">
-        <v>6.44</v>
+        <v>6.41</v>
       </c>
       <c r="E267" s="3" t="inlineStr"/>
       <c r="F267" s="3">
@@ -13274,7 +13274,7 @@
         <v>302</v>
       </c>
       <c r="D268" s="3" t="n">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="E268" s="3" t="inlineStr"/>
       <c r="F268" s="3">
@@ -13304,10 +13304,10 @@
         <v>33</v>
       </c>
       <c r="D269" s="3" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E269" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F269" s="3">
         <f>IF(B269:B477="common", 4, IF(B269:B477="uncommon", 3, IF(B269:B477="rare", 0.792892156862745, 1)))</f>
@@ -13336,7 +13336,7 @@
         <v>1362</v>
       </c>
       <c r="D270" s="3" t="n">
-        <v>2.39</v>
+        <v>2.12</v>
       </c>
       <c r="E270" s="3" t="inlineStr"/>
       <c r="F270" s="3">
@@ -13396,7 +13396,7 @@
         <v>1440</v>
       </c>
       <c r="D272" s="3" t="n">
-        <v>103.51</v>
+        <v>98.34999999999999</v>
       </c>
       <c r="E272" s="3" t="inlineStr"/>
       <c r="F272" s="3">
@@ -13426,7 +13426,7 @@
         <v>161</v>
       </c>
       <c r="D273" s="3" t="n">
-        <v>0.74</v>
+        <v>0.66</v>
       </c>
       <c r="E273" s="3" t="inlineStr"/>
       <c r="F273" s="3">
@@ -13456,10 +13456,10 @@
         <v>33</v>
       </c>
       <c r="D274" s="3" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="E274" s="3" t="n">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="F274" s="3">
         <f>IF(B274:B482="common", 4, IF(B274:B482="uncommon", 3, IF(B274:B482="rare", 0.792892156862745, 1)))</f>
@@ -13488,7 +13488,7 @@
         <v>1362</v>
       </c>
       <c r="D275" s="3" t="n">
-        <v>2.87</v>
+        <v>2.95</v>
       </c>
       <c r="E275" s="3" t="inlineStr"/>
       <c r="F275" s="3">
@@ -13518,7 +13518,7 @@
         <v>302</v>
       </c>
       <c r="D276" s="3" t="n">
-        <v>0.5</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E276" s="3" t="inlineStr"/>
       <c r="F276" s="3">
@@ -13548,10 +13548,10 @@
         <v>33</v>
       </c>
       <c r="D277" s="3" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="E277" s="3" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="F277" s="3">
         <f>IF(B277:B485="common", 4, IF(B277:B485="uncommon", 3, IF(B277:B485="rare", 0.792892156862745, 1)))</f>
@@ -13580,7 +13580,7 @@
         <v>302</v>
       </c>
       <c r="D278" s="3" t="n">
-        <v>0.4</v>
+        <v>0.46</v>
       </c>
       <c r="E278" s="3" t="inlineStr"/>
       <c r="F278" s="3">
@@ -13610,10 +13610,10 @@
         <v>46</v>
       </c>
       <c r="D279" s="3" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="E279" s="3" t="n">
-        <v>0.1</v>
+        <v>0.31</v>
       </c>
       <c r="F279" s="3">
         <f>IF(B279:B487="common", 4, IF(B279:B487="uncommon", 3, IF(B279:B487="rare", 0.792892156862745, 1)))</f>
@@ -13642,7 +13642,7 @@
         <v>1362</v>
       </c>
       <c r="D280" s="3" t="n">
-        <v>14.4</v>
+        <v>14.01</v>
       </c>
       <c r="E280" s="3" t="inlineStr"/>
       <c r="F280" s="3">
@@ -13672,7 +13672,7 @@
         <v>302</v>
       </c>
       <c r="D281" s="3" t="n">
-        <v>0.53</v>
+        <v>0.57</v>
       </c>
       <c r="E281" s="3" t="inlineStr"/>
       <c r="F281" s="3">
@@ -13702,10 +13702,10 @@
         <v>21</v>
       </c>
       <c r="D282" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="E282" s="3" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="F282" s="3">
         <f>IF(B282:B490="common", 4, IF(B282:B490="uncommon", 3, IF(B282:B490="rare", 0.792892156862745, 1)))</f>
@@ -13734,7 +13734,7 @@
         <v>1362</v>
       </c>
       <c r="D283" s="3" t="n">
-        <v>15.76</v>
+        <v>14.66</v>
       </c>
       <c r="E283" s="3" t="inlineStr"/>
       <c r="F283" s="3">
@@ -13764,7 +13764,7 @@
         <v>302</v>
       </c>
       <c r="D284" s="3" t="n">
-        <v>0.61</v>
+        <v>0.46</v>
       </c>
       <c r="E284" s="3" t="inlineStr"/>
       <c r="F284" s="3">
@@ -13794,7 +13794,7 @@
         <v>1440</v>
       </c>
       <c r="D285" s="3" t="n">
-        <v>217.7</v>
+        <v>190.9</v>
       </c>
       <c r="E285" s="3" t="inlineStr"/>
       <c r="F285" s="3">
@@ -13824,10 +13824,10 @@
         <v>46</v>
       </c>
       <c r="D286" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E286" s="3" t="n">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="F286" s="3">
         <f>IF(B286:B494="common", 4, IF(B286:B494="uncommon", 3, IF(B286:B494="rare", 0.792892156862745, 1)))</f>
@@ -13856,7 +13856,7 @@
         <v>302</v>
       </c>
       <c r="D287" s="3" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E287" s="3" t="inlineStr"/>
       <c r="F287" s="3">
@@ -13886,7 +13886,7 @@
         <v>106</v>
       </c>
       <c r="D288" s="3" t="n">
-        <v>0.41</v>
+        <v>0.36</v>
       </c>
       <c r="E288" s="3" t="inlineStr"/>
       <c r="F288" s="3">
@@ -13916,7 +13916,7 @@
         <v>1440</v>
       </c>
       <c r="D289" s="3" t="n">
-        <v>53.09</v>
+        <v>47.45</v>
       </c>
       <c r="E289" s="3" t="inlineStr"/>
       <c r="F289" s="3">
@@ -13946,7 +13946,7 @@
         <v>128</v>
       </c>
       <c r="D290" s="3" t="n">
-        <v>0.44</v>
+        <v>0.27</v>
       </c>
       <c r="E290" s="3" t="inlineStr"/>
       <c r="F290" s="3">
@@ -13976,10 +13976,10 @@
         <v>33</v>
       </c>
       <c r="D291" s="3" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="E291" s="3" t="n">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
       <c r="F291" s="3">
         <f>IF(B291:B499="common", 4, IF(B291:B499="uncommon", 3, IF(B291:B499="rare", 0.792892156862745, 1)))</f>
@@ -14008,7 +14008,7 @@
         <v>1362</v>
       </c>
       <c r="D292" s="3" t="n">
-        <v>8.43</v>
+        <v>8.24</v>
       </c>
       <c r="E292" s="3" t="inlineStr"/>
       <c r="F292" s="3">
@@ -14038,7 +14038,7 @@
         <v>302</v>
       </c>
       <c r="D293" s="3" t="n">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="E293" s="3" t="inlineStr"/>
       <c r="F293" s="3">
@@ -14068,10 +14068,10 @@
         <v>33</v>
       </c>
       <c r="D294" s="3" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="E294" s="3" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F294" s="3">
         <f>IF(B294:B502="common", 4, IF(B294:B502="uncommon", 3, IF(B294:B502="rare", 0.792892156862745, 1)))</f>
@@ -14100,7 +14100,7 @@
         <v>1362</v>
       </c>
       <c r="D295" s="3" t="n">
-        <v>3.38</v>
+        <v>3.49</v>
       </c>
       <c r="E295" s="3" t="inlineStr"/>
       <c r="F295" s="3">
@@ -14130,7 +14130,7 @@
         <v>302</v>
       </c>
       <c r="D296" s="3" t="n">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="E296" s="3" t="inlineStr"/>
       <c r="F296" s="3">
@@ -14160,10 +14160,10 @@
         <v>33</v>
       </c>
       <c r="D297" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="E297" s="3" t="n">
-        <v>0.14</v>
+        <v>0.1</v>
       </c>
       <c r="F297" s="3">
         <f>IF(B297:B505="common", 4, IF(B297:B505="uncommon", 3, IF(B297:B505="rare", 0.792892156862745, 1)))</f>
@@ -14192,7 +14192,7 @@
         <v>1362</v>
       </c>
       <c r="D298" s="3" t="n">
-        <v>8.5</v>
+        <v>7.88</v>
       </c>
       <c r="E298" s="3" t="inlineStr"/>
       <c r="F298" s="3">
@@ -14222,7 +14222,7 @@
         <v>302</v>
       </c>
       <c r="D299" s="3" t="n">
-        <v>0.39</v>
+        <v>0.35</v>
       </c>
       <c r="E299" s="3" t="inlineStr"/>
       <c r="F299" s="3">
@@ -14252,10 +14252,10 @@
         <v>33</v>
       </c>
       <c r="D300" s="3" t="n">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="E300" s="3" t="n">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F300" s="3">
         <f>IF(B300:B508="common", 4, IF(B300:B508="uncommon", 3, IF(B300:B508="rare", 0.792892156862745, 1)))</f>
@@ -14284,7 +14284,7 @@
         <v>1362</v>
       </c>
       <c r="D301" s="3" t="n">
-        <v>2.71</v>
+        <v>2.35</v>
       </c>
       <c r="E301" s="3" t="inlineStr"/>
       <c r="F301" s="3">
@@ -14314,7 +14314,7 @@
         <v>302</v>
       </c>
       <c r="D302" s="3" t="n">
-        <v>0.43</v>
+        <v>0.54</v>
       </c>
       <c r="E302" s="3" t="inlineStr"/>
       <c r="F302" s="3">
@@ -14344,10 +14344,10 @@
         <v>46</v>
       </c>
       <c r="D303" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E303" s="3" t="n">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F303" s="3">
         <f>IF(B303:B511="common", 4, IF(B303:B511="uncommon", 3, IF(B303:B511="rare", 0.792892156862745, 1)))</f>
@@ -14376,7 +14376,7 @@
         <v>1362</v>
       </c>
       <c r="D304" s="3" t="n">
-        <v>4.74</v>
+        <v>5.03</v>
       </c>
       <c r="E304" s="3" t="inlineStr"/>
       <c r="F304" s="3">
@@ -14406,7 +14406,7 @@
         <v>302</v>
       </c>
       <c r="D305" s="3" t="n">
-        <v>0.77</v>
+        <v>0.63</v>
       </c>
       <c r="E305" s="3" t="inlineStr"/>
       <c r="F305" s="3">
@@ -14436,10 +14436,10 @@
         <v>46</v>
       </c>
       <c r="D306" s="3" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E306" s="3" t="n">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="F306" s="3">
         <f>IF(B306:B514="common", 4, IF(B306:B514="uncommon", 3, IF(B306:B514="rare", 0.792892156862745, 1)))</f>
@@ -14468,7 +14468,7 @@
         <v>1362</v>
       </c>
       <c r="D307" s="3" t="n">
-        <v>3.68</v>
+        <v>2.81</v>
       </c>
       <c r="E307" s="3" t="inlineStr"/>
       <c r="F307" s="3">
@@ -14498,7 +14498,7 @@
         <v>302</v>
       </c>
       <c r="D308" s="3" t="n">
-        <v>0.45</v>
+        <v>0.36</v>
       </c>
       <c r="E308" s="3" t="inlineStr"/>
       <c r="F308" s="3">
@@ -14528,7 +14528,7 @@
         <v>106</v>
       </c>
       <c r="D309" s="3" t="n">
-        <v>0.7</v>
+        <v>0.99</v>
       </c>
       <c r="E309" s="3" t="inlineStr"/>
       <c r="F309" s="3">
@@ -14558,7 +14558,7 @@
         <v>128</v>
       </c>
       <c r="D310" s="3" t="n">
-        <v>0.52</v>
+        <v>0.72</v>
       </c>
       <c r="E310" s="3" t="inlineStr"/>
       <c r="F310" s="3">
@@ -14588,7 +14588,7 @@
         <v>46</v>
       </c>
       <c r="D311" s="3" t="n">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="E311" s="3" t="n">
         <v>0.09</v>
@@ -14620,7 +14620,7 @@
         <v>1362</v>
       </c>
       <c r="D312" s="3" t="n">
-        <v>2.02</v>
+        <v>2.03</v>
       </c>
       <c r="E312" s="3" t="inlineStr"/>
       <c r="F312" s="3">
@@ -14680,10 +14680,10 @@
         <v>33</v>
       </c>
       <c r="D314" s="3" t="n">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E314" s="3" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F314" s="3">
         <f>IF(B314:B522="common", 4, IF(B314:B522="uncommon", 3, IF(B314:B522="rare", 0.792892156862745, 1)))</f>
@@ -14712,7 +14712,7 @@
         <v>1362</v>
       </c>
       <c r="D315" s="3" t="n">
-        <v>18.13</v>
+        <v>16.97</v>
       </c>
       <c r="E315" s="3" t="inlineStr"/>
       <c r="F315" s="3">
@@ -14742,7 +14742,7 @@
         <v>302</v>
       </c>
       <c r="D316" s="3" t="n">
-        <v>0.78</v>
+        <v>0.85</v>
       </c>
       <c r="E316" s="3" t="inlineStr"/>
       <c r="F316" s="3">
@@ -14772,10 +14772,10 @@
         <v>21</v>
       </c>
       <c r="D317" s="3" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="E317" s="3" t="n">
-        <v>0.23</v>
+        <v>0.29</v>
       </c>
       <c r="F317" s="3">
         <f>IF(B317:B525="common", 4, IF(B317:B525="uncommon", 3, IF(B317:B525="rare", 0.792892156862745, 1)))</f>
@@ -14804,7 +14804,7 @@
         <v>1362</v>
       </c>
       <c r="D318" s="3" t="n">
-        <v>46.51</v>
+        <v>45.01</v>
       </c>
       <c r="E318" s="3" t="inlineStr"/>
       <c r="F318" s="3">
@@ -14834,7 +14834,7 @@
         <v>302</v>
       </c>
       <c r="D319" s="3" t="n">
-        <v>1.54</v>
+        <v>1.78</v>
       </c>
       <c r="E319" s="3" t="inlineStr"/>
       <c r="F319" s="3">
@@ -14864,7 +14864,7 @@
         <v>106</v>
       </c>
       <c r="D320" s="3" t="n">
-        <v>2.64</v>
+        <v>1.94</v>
       </c>
       <c r="E320" s="3" t="inlineStr"/>
       <c r="F320" s="3">
@@ -14894,7 +14894,7 @@
         <v>1440</v>
       </c>
       <c r="D321" s="3" t="n">
-        <v>485.86</v>
+        <v>450.56</v>
       </c>
       <c r="E321" s="3" t="inlineStr"/>
       <c r="F321" s="3">
@@ -14924,7 +14924,7 @@
         <v>106</v>
       </c>
       <c r="D322" s="3" t="n">
-        <v>1.45</v>
+        <v>1.41</v>
       </c>
       <c r="E322" s="3" t="inlineStr"/>
       <c r="F322" s="3">
@@ -14954,7 +14954,7 @@
         <v>1440</v>
       </c>
       <c r="D323" s="3" t="n">
-        <v>31.43</v>
+        <v>28.95</v>
       </c>
       <c r="E323" s="3" t="inlineStr"/>
       <c r="F323" s="3">
@@ -14984,7 +14984,7 @@
         <v>900</v>
       </c>
       <c r="D324" s="3" t="n">
-        <v>9.49</v>
+        <v>8.91</v>
       </c>
       <c r="E324" s="3" t="inlineStr"/>
       <c r="F324" s="3">
@@ -15014,10 +15014,10 @@
         <v>33</v>
       </c>
       <c r="D325" s="3" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="E325" s="3" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F325" s="3">
         <f>IF(B325:B533="common", 4, IF(B325:B533="uncommon", 3, IF(B325:B533="rare", 0.792892156862745, 1)))</f>
@@ -15046,7 +15046,7 @@
         <v>302</v>
       </c>
       <c r="D326" s="3" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="E326" s="3" t="inlineStr"/>
       <c r="F326" s="3">
@@ -15076,7 +15076,7 @@
         <v>106</v>
       </c>
       <c r="D327" s="3" t="n">
-        <v>1.1</v>
+        <v>0.99</v>
       </c>
       <c r="E327" s="3" t="inlineStr"/>
       <c r="F327" s="3">
@@ -15106,7 +15106,7 @@
         <v>1440</v>
       </c>
       <c r="D328" s="3" t="n">
-        <v>49.19</v>
+        <v>48.2</v>
       </c>
       <c r="E328" s="3" t="inlineStr"/>
       <c r="F328" s="3">
@@ -15136,7 +15136,7 @@
         <v>900</v>
       </c>
       <c r="D329" s="3" t="n">
-        <v>11.65</v>
+        <v>10.36</v>
       </c>
       <c r="E329" s="3" t="inlineStr"/>
       <c r="F329" s="3">
@@ -15166,7 +15166,7 @@
         <v>128</v>
       </c>
       <c r="D330" s="3" t="n">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="E330" s="3" t="inlineStr"/>
       <c r="F330" s="3">
@@ -15196,7 +15196,7 @@
         <v>161</v>
       </c>
       <c r="D331" s="3" t="n">
-        <v>0.59</v>
+        <v>0.54</v>
       </c>
       <c r="E331" s="3" t="inlineStr"/>
       <c r="F331" s="3">
@@ -15226,7 +15226,7 @@
         <v>106</v>
       </c>
       <c r="D332" s="3" t="n">
-        <v>0.49</v>
+        <v>0.66</v>
       </c>
       <c r="E332" s="3" t="inlineStr"/>
       <c r="F332" s="3">
@@ -15256,10 +15256,10 @@
         <v>21</v>
       </c>
       <c r="D333" s="3" t="n">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="E333" s="3" t="n">
-        <v>0.36</v>
+        <v>0.29</v>
       </c>
       <c r="F333" s="3">
         <f>IF(B333:B541="common", 4, IF(B333:B541="uncommon", 3, IF(B333:B541="rare", 0.792892156862745, 1)))</f>
@@ -15288,7 +15288,7 @@
         <v>1362</v>
       </c>
       <c r="D334" s="3" t="n">
-        <v>90.63</v>
+        <v>90.61</v>
       </c>
       <c r="E334" s="3" t="inlineStr"/>
       <c r="F334" s="3">
@@ -15318,7 +15318,7 @@
         <v>302</v>
       </c>
       <c r="D335" s="3" t="n">
-        <v>3.71</v>
+        <v>3.7</v>
       </c>
       <c r="E335" s="3" t="inlineStr"/>
       <c r="F335" s="3">
@@ -15348,7 +15348,7 @@
         <v>106</v>
       </c>
       <c r="D336" s="3" t="n">
-        <v>4.93</v>
+        <v>4.89</v>
       </c>
       <c r="E336" s="3" t="inlineStr"/>
       <c r="F336" s="3">
@@ -15378,7 +15378,7 @@
         <v>1440</v>
       </c>
       <c r="D337" s="3" t="n">
-        <v>1224.45</v>
+        <v>1168.88</v>
       </c>
       <c r="E337" s="3" t="inlineStr"/>
       <c r="F337" s="3">
@@ -15408,10 +15408,10 @@
         <v>21</v>
       </c>
       <c r="D338" s="3" t="n">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="E338" s="3" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F338" s="3">
         <f>IF(B338:B546="common", 4, IF(B338:B546="uncommon", 3, IF(B338:B546="rare", 0.792892156862745, 1)))</f>
@@ -15440,7 +15440,7 @@
         <v>1362</v>
       </c>
       <c r="D339" s="3" t="n">
-        <v>37.06</v>
+        <v>34.62</v>
       </c>
       <c r="E339" s="3" t="inlineStr"/>
       <c r="F339" s="3">
@@ -15470,7 +15470,7 @@
         <v>302</v>
       </c>
       <c r="D340" s="3" t="n">
-        <v>1.46</v>
+        <v>1.53</v>
       </c>
       <c r="E340" s="3" t="inlineStr"/>
       <c r="F340" s="3">
@@ -15500,7 +15500,7 @@
         <v>106</v>
       </c>
       <c r="D341" s="3" t="n">
-        <v>2.15</v>
+        <v>2.04</v>
       </c>
       <c r="E341" s="3" t="inlineStr"/>
       <c r="F341" s="3">
@@ -15530,7 +15530,7 @@
         <v>1440</v>
       </c>
       <c r="D342" s="3" t="n">
-        <v>276.12</v>
+        <v>262.19</v>
       </c>
       <c r="E342" s="3" t="inlineStr"/>
       <c r="F342" s="3">
@@ -15560,7 +15560,7 @@
         <v>900</v>
       </c>
       <c r="D343" s="3" t="n">
-        <v>7.58</v>
+        <v>7.94</v>
       </c>
       <c r="E343" s="3" t="inlineStr"/>
       <c r="F343" s="3">
@@ -15590,7 +15590,7 @@
         <v>106</v>
       </c>
       <c r="D344" s="3" t="n">
-        <v>0.47</v>
+        <v>0.5</v>
       </c>
       <c r="E344" s="3" t="inlineStr"/>
       <c r="F344" s="3">
@@ -15620,7 +15620,7 @@
         <v>1440</v>
       </c>
       <c r="D345" s="3" t="n">
-        <v>27.06</v>
+        <v>23.03</v>
       </c>
       <c r="E345" s="3" t="inlineStr"/>
       <c r="F345" s="3">
@@ -15650,7 +15650,7 @@
         <v>21</v>
       </c>
       <c r="D346" s="3" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E346" s="3" t="n">
         <v>0.1</v>
@@ -15682,7 +15682,7 @@
         <v>1362</v>
       </c>
       <c r="D347" s="3" t="n">
-        <v>9.289999999999999</v>
+        <v>8.18</v>
       </c>
       <c r="E347" s="3" t="inlineStr"/>
       <c r="F347" s="3">
@@ -15712,7 +15712,7 @@
         <v>302</v>
       </c>
       <c r="D348" s="3" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="E348" s="3" t="inlineStr"/>
       <c r="F348" s="3">
@@ -21266,7 +21266,7 @@
         </is>
       </c>
       <c r="B2" s="15" t="n">
-        <v>0.2443478260869565</v>
+        <v>0.2591304347826086</v>
       </c>
     </row>
     <row r="3">
@@ -21276,7 +21276,7 @@
         </is>
       </c>
       <c r="B3" s="15" t="n">
-        <v>0.2536363636363637</v>
+        <v>0.2481818181818182</v>
       </c>
     </row>
     <row r="4">
@@ -21286,7 +21286,7 @@
         </is>
       </c>
       <c r="B4" s="15" t="n">
-        <v>0.1215669515669515</v>
+        <v>0.1133433048433048</v>
       </c>
     </row>
     <row r="5">
@@ -21296,7 +21296,7 @@
         </is>
       </c>
       <c r="B5" s="15" t="n">
-        <v>0.9008236932149973</v>
+        <v>0.8590740040957431</v>
       </c>
     </row>
     <row r="6">
@@ -21306,7 +21306,7 @@
         </is>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.03203125</v>
+        <v>0.031953125</v>
       </c>
     </row>
     <row r="7">
@@ -21316,7 +21316,7 @@
         </is>
       </c>
       <c r="B7" s="15" t="n">
-        <v>0.2245695364238411</v>
+        <v>0.2102980132450331</v>
       </c>
     </row>
     <row r="8">
@@ -21326,7 +21326,7 @@
         </is>
       </c>
       <c r="B8" s="15" t="n">
-        <v>0.5477092511013216</v>
+        <v>0.5217327459618208</v>
       </c>
     </row>
     <row r="9">
@@ -21346,7 +21346,7 @@
         </is>
       </c>
       <c r="B10" s="15" t="n">
-        <v>3.675895833333333</v>
+        <v>3.414979166666667</v>
       </c>
     </row>
     <row r="11">
@@ -21356,7 +21356,7 @@
         </is>
       </c>
       <c r="B11" s="15" t="n">
-        <v>0.4623584905660377</v>
+        <v>0.4056603773584905</v>
       </c>
     </row>
     <row r="12">
@@ -21366,7 +21366,7 @@
         </is>
       </c>
       <c r="B12" s="15" t="n">
-        <v>0.09033333333333332</v>
+        <v>0.08163333333333332</v>
       </c>
     </row>
     <row r="13">
@@ -21376,7 +21376,7 @@
         </is>
       </c>
       <c r="B13" s="15" t="n">
-        <v>0.06726708074534161</v>
+        <v>0.05906832298136646</v>
       </c>
     </row>
     <row r="14">
@@ -21406,7 +21406,7 @@
         </is>
       </c>
       <c r="B16" s="15" t="n">
-        <v>5.100164775503209</v>
+        <v>4.725325084546711</v>
       </c>
     </row>
     <row r="17">
@@ -21416,7 +21416,7 @@
         </is>
       </c>
       <c r="B17" s="15" t="n">
-        <v>6.620539610008477</v>
+        <v>6.205054646450185</v>
       </c>
     </row>
     <row r="18">
@@ -21426,7 +21426,7 @@
         </is>
       </c>
       <c r="B18" s="15" t="n">
-        <v>-4.479460389991522</v>
+        <v>-3.664945353549814</v>
       </c>
     </row>
     <row r="19">
@@ -21436,7 +21436,7 @@
         </is>
       </c>
       <c r="B19" s="16" t="n">
-        <v>0.5964450099106736</v>
+        <v>0.6286782823151151</v>
       </c>
     </row>
     <row r="20">
@@ -21446,7 +21446,7 @@
         </is>
       </c>
       <c r="B20" s="17" t="n">
-        <v>-0.4035549900893264</v>
+        <v>-0.3713217176848849</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
updates for more dynamic calcs
</commit_message>
<xml_diff>
--- a/excelDocs/prismaticEvolution/pokemon_data.xlsx
+++ b/excelDocs/prismaticEvolution/pokemon_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVRCalculator\excelDocs\prismaticEvolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DC19CF-6B69-45D7-A06F-0DCE18BF0A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D059E375-D8AF-4311-B508-BB44B1B8376F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="825" windowWidth="25260" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="1605" windowWidth="25260" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1656,7 +1656,7 @@
   <dimension ref="A1:AZ1263"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="G2" s="3">
         <f>SUM(H2:H12)</f>
-        <v>6.2049401379544449</v>
+        <v>5.8404109180972172</v>
       </c>
       <c r="H2" s="3">
         <f>4*SUMPRODUCT(
@@ -1930,8 +1930,8 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
-        <f>1.517547 * SUMPRODUCT((C2:C348&lt;&gt;"") * (E2:E348&lt;&gt;"") * (E2:E348 / C2:C348))</f>
-        <v>0.85908851472902015</v>
+        <f>SUM(E2:E210) * (1.88541666666666 / COUNTA(E2:E210))</f>
+        <v>0.49455929487179312</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -14719,7 +14719,7 @@
       </c>
       <c r="E322" s="3"/>
       <c r="F322" s="3">
-        <f t="shared" ref="F322:F385" si="5">IF(B322:B530="common", 4, IF(B322:B530="uncommon", 3, IF(B322:B530="rare", 0.792892156862745, 1)))</f>
+        <f t="shared" ref="F322:F348" si="5">IF(B322:B530="common", 4, IF(B322:B530="uncommon", 3, IF(B322:B530="rare", 0.792892156862745, 1)))</f>
         <v>1</v>
       </c>
       <c r="I322" s="3"/>

</xml_diff>

<commit_message>
God pack and Demi god pack logic working for both set with and without
</commit_message>
<xml_diff>
--- a/excelDocs/prismaticEvolution/pokemon_data.xlsx
+++ b/excelDocs/prismaticEvolution/pokemon_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EVRCalculator\excelDocs\prismaticEvolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D059E375-D8AF-4311-B508-BB44B1B8376F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D2FC64-FC3E-4CA2-8D73-A5082873B8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1605" windowWidth="25260" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1350,6 +1350,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,13 +1755,11 @@
       </c>
       <c r="G2" s="3">
         <f>SUM(H2:H12)</f>
-        <v>5.8404109180972172</v>
+        <v>5.6911311287699791</v>
       </c>
       <c r="H2" s="3">
         <f>4*SUMPRODUCT(
   (B2:B348="common") *
-  ISERROR(SEARCH("Master Ball Pattern", A2:A348)) *
-  ISERROR(SEARCH("Poke Ball Pattern", A2:A348)) *
   D2:D348 / C2:C348
 )</f>
         <v>0.25913043478260861</v>
@@ -1818,12 +1819,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <f>SUM(D98, D101, D107,D128, D144,D198,D215, D321, D337, D342) * 0.0005</f>
+        <v>1.73509</v>
+      </c>
       <c r="H3" s="3">
         <f>3*SUMPRODUCT(
   (ISNUMBER(SEARCH("uncommon", B2:B348))) *
-  ISERROR(SEARCH("Master Ball Pattern", A2:A348)) *
-  ISERROR(SEARCH("Poke Ball Pattern", A2:A348)) *
   D2:D348 / C2:C348
 )</f>
         <v>0.24818181818181811</v>
@@ -1877,8 +1879,6 @@
       <c r="H4" s="3">
         <f>0.75*SUMPRODUCT(
   (B2:B348="Rare") *
-  ISERROR(SEARCH("Master Ball Pattern", A2:A348)) *
-  ISERROR(SEARCH("Poke Ball Pattern", A2:A348)) *
   D2:D348  / C2:C348
 )</f>
         <v>0.11321428571428574</v>
@@ -1930,8 +1930,8 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
-        <f>SUM(E2:E210) * (1.88541666666666 / COUNTA(E2:E210))</f>
-        <v>0.49455929487179312</v>
+        <f>SUM(E2:E348) * (1.517547 / COUNTA(E2:E348))</f>
+        <v>0.34527950554455455</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -2435,7 +2435,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3">
+        <f>SUM(E2:E348)</f>
+        <v>22.980000000000008</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -2482,7 +2485,9 @@
         <v>1</v>
       </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3">
+        <v>1.8854166666666601</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -2529,7 +2534,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3">
+        <f>COUNTA(E2:E348)</f>
+        <v>101</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2672,7 +2680,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3">
+        <f xml:space="preserve"> H15 *(H16 / H17)</f>
+        <v>0.42897896039603822</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2817,7 +2828,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="13"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -3105,7 +3116,10 @@
         <v>0.79289215686274495</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3">
+        <f xml:space="preserve"> H9 * 3 * 3/2000</f>
+        <v>1.5367406250000002E-2</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>

</xml_diff>

<commit_message>
Refactor get_config_for_set function to return matched keys and improve error handling for set name resolution
</commit_message>
<xml_diff>
--- a/excelDocs/prismaticEvolution/pokemon_data.xlsx
+++ b/excelDocs/prismaticEvolution/pokemon_data.xlsx
@@ -21270,7 +21270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21286,7 +21286,7 @@
     <row r="1">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>Metric</t>
+          <t>Summary Metric</t>
         </is>
       </c>
       <c r="B1" s="13" t="inlineStr">
@@ -21301,8 +21301,8 @@
           <t>ev_common_total</t>
         </is>
       </c>
-      <c r="B2" s="15" t="n">
-        <v>0.2278260869565217</v>
+      <c r="B2" s="14" t="n">
+        <v>0.2069565217391304</v>
       </c>
     </row>
     <row r="3">
@@ -21311,8 +21311,8 @@
           <t>ev_uncommon_total</t>
         </is>
       </c>
-      <c r="B3" s="15" t="n">
-        <v>0.2018181818181818</v>
+      <c r="B3" s="14" t="n">
+        <v>0.2045454545454546</v>
       </c>
     </row>
     <row r="4">
@@ -21321,8 +21321,8 @@
           <t>ev_rare_total</t>
         </is>
       </c>
-      <c r="B4" s="15" t="n">
-        <v>0.1314713064713065</v>
+      <c r="B4" s="14" t="n">
+        <v>0.1213858363858364</v>
       </c>
     </row>
     <row r="5">
@@ -21331,8 +21331,8 @@
           <t>ev_reverse_total</t>
         </is>
       </c>
-      <c r="B5" s="15" t="n">
-        <v>0.2267948717948718</v>
+      <c r="B5" s="14" t="n">
+        <v>0.2186302564102564</v>
       </c>
     </row>
     <row r="6">
@@ -21341,8 +21341,8 @@
           <t>ev_ace_spec_total</t>
         </is>
       </c>
-      <c r="B6" s="15" t="n">
-        <v>0.02515625</v>
+      <c r="B6" s="14" t="n">
+        <v>0.02171875</v>
       </c>
     </row>
     <row r="7">
@@ -21351,8 +21351,8 @@
           <t>ev_pokeball_total</t>
         </is>
       </c>
-      <c r="B7" s="15" t="n">
-        <v>0.1762582781456954</v>
+      <c r="B7" s="14" t="n">
+        <v>0.136953642384106</v>
       </c>
     </row>
     <row r="8">
@@ -21361,8 +21361,8 @@
           <t>ev_master_ball_total</t>
         </is>
       </c>
-      <c r="B8" s="15" t="n">
-        <v>0.4267767988252569</v>
+      <c r="B8" s="14" t="n">
+        <v>0.3463069016152716</v>
       </c>
     </row>
     <row r="9">
@@ -21371,7 +21371,7 @@
           <t>ev_IR_total</t>
         </is>
       </c>
-      <c r="B9" s="15" t="n">
+      <c r="B9" s="14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21381,8 +21381,8 @@
           <t>ev_SIR_total</t>
         </is>
       </c>
-      <c r="B10" s="15" t="n">
-        <v>2.538333333333333</v>
+      <c r="B10" s="14" t="n">
+        <v>2.662319444444444</v>
       </c>
     </row>
     <row r="11">
@@ -21391,8 +21391,8 @@
           <t>ev_double_rare_total</t>
         </is>
       </c>
-      <c r="B11" s="15" t="n">
-        <v>0.4316981132075472</v>
+      <c r="B11" s="14" t="n">
+        <v>0.3275471698113208</v>
       </c>
     </row>
     <row r="12">
@@ -21401,8 +21401,8 @@
           <t>ev_hyper_rare_total</t>
         </is>
       </c>
-      <c r="B12" s="15" t="n">
-        <v>0.0919</v>
+      <c r="B12" s="14" t="n">
+        <v>0.07271111111111112</v>
       </c>
     </row>
     <row r="13">
@@ -21411,8 +21411,8 @@
           <t>ev_ultra_rare_total</t>
         </is>
       </c>
-      <c r="B13" s="15" t="n">
-        <v>0.06055900621118013</v>
+      <c r="B13" s="14" t="n">
+        <v>0.04571428571428571</v>
       </c>
     </row>
     <row r="14">
@@ -21442,7 +21442,7 @@
         </is>
       </c>
       <c r="B16" s="14" t="n">
-        <v>4.538592226763895</v>
+        <v>4.364789374161218</v>
       </c>
     </row>
     <row r="17">
@@ -21452,7 +21452,7 @@
         </is>
       </c>
       <c r="B17" s="14" t="n">
-        <v>1.266365</v>
+        <v>1.39661</v>
       </c>
     </row>
     <row r="18">
@@ -21462,7 +21462,7 @@
         </is>
       </c>
       <c r="B18" s="14" t="n">
-        <v>0.5146569664031621</v>
+        <v>0.5397369404644269</v>
       </c>
     </row>
     <row r="19">
@@ -21472,296 +21472,368 @@
         </is>
       </c>
       <c r="B19" s="14" t="n">
-        <v>6.319614193167057</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="14" t="inlineStr">
-        <is>
-          <t>net_value</t>
-        </is>
-      </c>
-      <c r="B20" s="15" t="n">
-        <v>-2.707817200000001</v>
+        <v>6.301136314625644</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="14" t="inlineStr">
-        <is>
-          <t>opening_pack_roi</t>
-        </is>
-      </c>
-      <c r="B21" s="14" t="n">
-        <v>0.6787879952550414</v>
+      <c r="A21" s="13" t="inlineStr">
+        <is>
+          <t>Results Metric</t>
+        </is>
+      </c>
+      <c r="B21" s="13" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="14" t="inlineStr">
         <is>
-          <t>opening_pack_roi_percent</t>
+          <t>total_manual_ev</t>
         </is>
       </c>
       <c r="B22" s="14" t="n">
-        <v>-32.12120047449586</v>
+        <v>6.301136314625644</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="14" t="inlineStr">
         <is>
-          <t>no_hit_probability_percentage</t>
-        </is>
-      </c>
-      <c r="B23" s="16" t="n">
-        <v>0.4598075322602833</v>
+          <t>acutal_simulated_ev</t>
+        </is>
+      </c>
+      <c r="B23" s="14" t="n">
+        <v>5.6661488</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="14" t="inlineStr">
         <is>
+          <t>pack_price</t>
+        </is>
+      </c>
+      <c r="B24" s="14" t="n">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="14" t="inlineStr">
+        <is>
           <t>hit_probability_percentage</t>
         </is>
       </c>
-      <c r="B24" s="16" t="n">
-        <v>0.5401924677397167</v>
+      <c r="B25" s="14" t="n">
+        <v>54.01924677397167</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="inlineStr">
+      <c r="A26" s="14" t="inlineStr">
+        <is>
+          <t>no_hit_probability_percentage</t>
+        </is>
+      </c>
+      <c r="B26" s="14" t="n">
+        <v>45.98075322602833</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="14" t="inlineStr">
+        <is>
+          <t>net_value</t>
+        </is>
+      </c>
+      <c r="B27" s="14" t="n">
+        <v>-3.0138512</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="14" t="inlineStr">
+        <is>
+          <t>opening_pack_roi</t>
+        </is>
+      </c>
+      <c r="B28" s="14" t="n">
+        <v>0.6527821198156682</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="14" t="inlineStr">
+        <is>
+          <t>opening_pack_roi_percent</t>
+        </is>
+      </c>
+      <c r="B29" s="14" t="n">
+        <v>-34.72178801843317</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="13" t="inlineStr">
         <is>
           <t>Simulation Metric</t>
         </is>
       </c>
-      <c r="B26" s="13" t="inlineStr">
+      <c r="B31" s="13" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Mean Value</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>5.722182799999999</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Standard Deviation</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>64.89606525161123</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Minimum Value</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Maximum Value</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>2532.73</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>5th</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0.71</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>25th</t>
+          <t>Mean Value</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.89</v>
+        <v>5.6661488</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>50th (median)</t>
+          <t>Standard Deviation</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1.12</v>
+        <v>70.07639828971134</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>75th</t>
+          <t>Minimum Value</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.73</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>90th</t>
+          <t>Maximum Value</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3.32</v>
+        <v>2793.22</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>95th</t>
+          <t>5th</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>7.770499999999884</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>99th</t>
+          <t>25th</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>78.55000000000001</v>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>50th (median)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1.03</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="13" t="inlineStr">
-        <is>
-          <t>Top 10 Most Expensive Hits</t>
-        </is>
-      </c>
-      <c r="B39" s="13" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="C39" s="13" t="inlineStr">
-        <is>
-          <t>Effective Pull Rate</t>
-        </is>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>75th</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1.49</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Umbreon ex - 161/131</t>
+          <t>90th</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>919.79</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sylveon ex - 156/131</t>
+          <t>95th</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>331.95</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Leafeon ex - 144/131</t>
+          <t>99th</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>266.35</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Espeon ex - 155/131</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>208.99</v>
+        <v>68.73999999999999</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Vaporeon ex - 149/131</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>196.36</v>
+      <c r="A44" s="13" t="inlineStr">
+        <is>
+          <t>Top 10 Most Expensive Hits</t>
+        </is>
+      </c>
+      <c r="B44" s="13" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C44" s="13" t="inlineStr">
+        <is>
+          <t>Effective Pull Rate</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Roaring Moon ex</t>
+          <t>Umbreon ex - 161/131</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>194.84</v>
+        <v>1119.08</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1440</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Glaceon ex - 150/131</t>
+          <t>Sylveon ex - 156/131</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>172.9</v>
+        <v>334.99</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1440</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Flareon ex - 146/131</t>
+          <t>Leafeon ex - 144/131</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>163.68</v>
+        <v>263.09</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1440</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Jolteon ex - 153/131</t>
+          <t>Espeon ex - 155/131</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>149.83</v>
+        <v>207.51</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1440</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>Vaporeon ex - 149/131</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>206.67</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Glaceon ex - 150/131</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>205.76</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Roaring Moon ex</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>182.46</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Flareon ex - 146/131</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>163.98</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Jolteon ex - 153/131</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>159.06</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>Eevee ex - 167/131</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>112.93</v>
+      <c r="B54" t="n">
+        <v>123.02</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor pack calculation logic and simulations
- Moved simulation code to a new structure under `src/simulations`.
- Introduced `PackCalculationOrchestrator` and `PackEVRSimulator` for better organization and clarity.
- Added `otherCalculations.py` for comprehensive pack metrics calculations.
- Implemented Monte Carlo simulation methods in `monteCarloSim.py`.
- Updated import paths and ensured backward compatibility with deprecated shims.
- Enhanced variance and standard deviation calculations for pack EV metrics.
- Updated Excel data files for `prismaticEvolution` and `scarletAndViolet151`.
</commit_message>
<xml_diff>
--- a/excelDocs/prismaticEvolution/pokemon_data.xlsx
+++ b/excelDocs/prismaticEvolution/pokemon_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2370" yWindow="2985" windowWidth="25260" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data'!$A$1:$L$210</definedName>
@@ -21504,7 +21504,7 @@
         </is>
       </c>
       <c r="B23" s="14" t="n">
-        <v>5.6661488</v>
+        <v>5.5066146</v>
       </c>
     </row>
     <row r="24">
@@ -21544,7 +21544,7 @@
         </is>
       </c>
       <c r="B27" s="14" t="n">
-        <v>-3.0138512</v>
+        <v>-3.1733854</v>
       </c>
     </row>
     <row r="28">
@@ -21554,7 +21554,7 @@
         </is>
       </c>
       <c r="B28" s="14" t="n">
-        <v>0.6527821198156682</v>
+        <v>0.6344026036866359</v>
       </c>
     </row>
     <row r="29">
@@ -21564,7 +21564,7 @@
         </is>
       </c>
       <c r="B29" s="14" t="n">
-        <v>-34.72178801843317</v>
+        <v>-36.55973963133641</v>
       </c>
     </row>
     <row r="31">
@@ -21586,7 +21586,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.6661488</v>
+        <v>5.5066146</v>
       </c>
     </row>
     <row r="33">
@@ -21596,7 +21596,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>70.07639828971134</v>
+        <v>69.05108769448216</v>
       </c>
     </row>
     <row r="34">
@@ -21606,7 +21606,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="35">
@@ -21636,7 +21636,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.85</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="38">
@@ -21676,7 +21676,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>6.35</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="42">
@@ -21686,7 +21686,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>68.73999999999999</v>
+        <v>68.70009999999995</v>
       </c>
     </row>
     <row r="44">

</xml_diff>